<commit_message>
Added deposit from Onno: up to March + April + May 2018
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -513,10 +513,10 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26:XFD26"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,7 +691,7 @@
         <v>80.03</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" ref="E10:E37" si="3">D9</f>
+        <f t="shared" ref="E10:E28" si="3">D9</f>
         <v>87.26</v>
       </c>
       <c r="F10" s="2">
@@ -1519,16 +1519,19 @@
         <f t="shared" si="6"/>
         <v>1362.98</v>
       </c>
+      <c r="K28" s="4">
+        <v>1800</v>
+      </c>
       <c r="M28" s="5">
         <v>1170</v>
       </c>
       <c r="O28" s="3">
         <f t="shared" si="8"/>
-        <v>1303.236666666666</v>
+        <v>-496.76333333333423</v>
       </c>
       <c r="P28" s="4">
         <f t="shared" si="9"/>
-        <v>1224.2333333333333</v>
+        <v>-575.76666666666665</v>
       </c>
       <c r="R28" s="5">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
Adding payment to landlord for May.
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -513,10 +513,10 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
+      <selection pane="bottomRight" activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,22 +691,22 @@
         <v>80.03</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" ref="E10:E28" si="3">D9</f>
+        <f t="shared" ref="E10:E30" si="3">D9</f>
         <v>87.26</v>
       </c>
       <c r="F10" s="2">
         <v>59.99</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G28" si="4">C10+E10+F10</f>
+        <f t="shared" ref="G10:G30" si="4">C10+E10+F10</f>
         <v>1272.25</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10:H28" si="5">G10/3</f>
+        <f t="shared" ref="H10:H30" si="5">G10/3</f>
         <v>424.08333333333331</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" ref="J10:J28" si="6">G10</f>
+        <f t="shared" ref="J10:J30" si="6">G10</f>
         <v>1272.25</v>
       </c>
       <c r="K10" s="4">
@@ -1485,11 +1485,11 @@
         <v>1564.5833333333326</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" ref="P27:P28" si="9">P26 + H27 - K27</f>
+        <f t="shared" ref="P27:P30" si="9">P26 + H27 - K27</f>
         <v>769.90666666666675</v>
       </c>
       <c r="R27" s="5">
-        <f t="shared" ref="R27:R28" si="10">R26 + H27 - M27</f>
+        <f t="shared" ref="R27:R30" si="10">R26 + H27 - M27</f>
         <v>795.6733333333334</v>
       </c>
     </row>
@@ -1500,6 +1500,9 @@
       <c r="C28" s="2">
         <v>1145</v>
       </c>
+      <c r="D28" s="2">
+        <v>177.54</v>
+      </c>
       <c r="E28" s="2">
         <f t="shared" si="3"/>
         <v>157.99</v>
@@ -1545,6 +1548,40 @@
       <c r="C29" s="2">
         <v>1145</v>
       </c>
+      <c r="D29" s="2">
+        <v>164.3</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="3"/>
+        <v>177.54</v>
+      </c>
+      <c r="F29" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="4"/>
+        <v>1382.53</v>
+      </c>
+      <c r="H29" s="6">
+        <f t="shared" si="5"/>
+        <v>460.84333333333331</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="6"/>
+        <v>1382.53</v>
+      </c>
+      <c r="O29" s="3">
+        <f>O28 + J29 - (H29 + K29+ L29 + M29)</f>
+        <v>424.92333333333244</v>
+      </c>
+      <c r="P29" s="4">
+        <f t="shared" si="9"/>
+        <v>-114.92333333333335</v>
+      </c>
+      <c r="R29" s="5">
+        <f t="shared" si="10"/>
+        <v>540.84333333333325</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
@@ -1552,6 +1589,37 @@
       </c>
       <c r="C30" s="2">
         <v>1145</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="3"/>
+        <v>164.3</v>
+      </c>
+      <c r="F30" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="4"/>
+        <v>1369.29</v>
+      </c>
+      <c r="H30" s="6">
+        <f t="shared" si="5"/>
+        <v>456.43</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="6"/>
+        <v>1369.29</v>
+      </c>
+      <c r="O30" s="3">
+        <f>O29 + J30 - (H30 + K30+ L30 + M30)</f>
+        <v>1337.7833333333324</v>
+      </c>
+      <c r="P30" s="4">
+        <f t="shared" si="9"/>
+        <v>341.50666666666666</v>
+      </c>
+      <c r="R30" s="5">
+        <f t="shared" si="10"/>
+        <v>997.27333333333331</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added nick's payment for april+may
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>January</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Nick Balance</t>
+  </si>
+  <si>
+    <t>&lt;-- This $80 Nick and Roy agreed was an initial programming error.</t>
   </si>
 </sst>
 </file>
@@ -510,13 +513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R30" sqref="R30"/>
+      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,6 +542,7 @@
     <col min="16" max="16" width="12.36328125" style="4" customWidth="1"/>
     <col min="17" max="17" width="12.453125" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="63.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -1004,7 +1008,7 @@
         <v>-0.99333333333345308</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1050,7 @@
         <v>394.00333333333322</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>4</v>
       </c>
@@ -1091,7 +1095,7 @@
         <v>-0.99666666666678339</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>433.70333333333332</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1185,7 @@
         <v>-6.6666666666606034E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1227,7 @@
         <v>418.99</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -1271,7 +1275,7 @@
         <v>-1.3333333333321207E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1317,7 @@
         <v>425.55</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +1362,7 @@
         <v>-57.370000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -1400,7 +1404,7 @@
         <v>389.30333333333334</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2018</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>843.96333333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -1493,7 +1497,7 @@
         <v>795.6733333333334</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -1540,8 +1544,11 @@
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -1583,7 +1590,7 @@
         <v>540.84333333333325</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -1609,9 +1616,12 @@
         <f t="shared" si="6"/>
         <v>1369.29</v>
       </c>
+      <c r="M30" s="5">
+        <v>1000</v>
+      </c>
       <c r="O30" s="3">
         <f>O29 + J30 - (H30 + K30+ L30 + M30)</f>
-        <v>1337.7833333333324</v>
+        <v>337.78333333333239</v>
       </c>
       <c r="P30" s="4">
         <f t="shared" si="9"/>
@@ -1619,10 +1629,10 @@
       </c>
       <c r="R30" s="5">
         <f t="shared" si="10"/>
-        <v>997.27333333333331</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+        <v>-2.7266666666666879</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -1630,7 +1640,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added column for chandler
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>January</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>&lt;-- This $80 Nick and Roy agreed was an initial programming error.</t>
+  </si>
+  <si>
+    <t>Chan Balance</t>
+  </si>
+  <si>
+    <t>Chan Paid</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -198,6 +204,7 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -513,13 +520,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -537,15 +544,16 @@
     <col min="11" max="11" width="9.453125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" style="2"/>
-    <col min="15" max="15" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.36328125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="12.453125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="63.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.08984375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.36328125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.54296875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="63.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -582,20 +590,26 @@
       <c r="M1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2016</v>
       </c>
@@ -603,32 +617,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -636,7 +650,7 @@
         <v>79.540000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -671,20 +685,20 @@
       <c r="L9" s="1">
         <v>422</v>
       </c>
-      <c r="O9" s="3">
-        <f t="shared" ref="O9:O26" si="0">O8 + J9 - (H9 + K9+ L9 + M9)</f>
+      <c r="P9" s="3">
+        <f>P8 + J9 - (H9 + K9+ L9 + M9)</f>
         <v>1.0199999999999818</v>
       </c>
-      <c r="P9" s="4">
-        <f t="shared" ref="P9:P26" si="1">P8 + H9 - K9</f>
+      <c r="Q9" s="4">
+        <f>Q8 + H9 - K9</f>
         <v>1.5099999999999909</v>
       </c>
-      <c r="Q9" s="1">
-        <f t="shared" ref="Q9:Q18" si="2">Q8 + H9 - L9</f>
+      <c r="R9" s="1">
+        <f>R8 + H9 - L9</f>
         <v>-0.49000000000000909</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -695,22 +709,22 @@
         <v>80.03</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" ref="E10:E30" si="3">D9</f>
+        <f t="shared" ref="E10:E31" si="0">D9</f>
         <v>87.26</v>
       </c>
       <c r="F10" s="2">
         <v>59.99</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G30" si="4">C10+E10+F10</f>
+        <f t="shared" ref="G10:G31" si="1">C10+E10+F10</f>
         <v>1272.25</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10:H30" si="5">G10/3</f>
+        <f t="shared" ref="H10:H31" si="2">G10/3</f>
         <v>424.08333333333331</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" ref="J10:J30" si="6">G10</f>
+        <f t="shared" ref="J10:J30" si="3">G10</f>
         <v>1272.25</v>
       </c>
       <c r="K10" s="4">
@@ -719,20 +733,20 @@
       <c r="L10" s="1">
         <v>424</v>
       </c>
-      <c r="O10" s="3">
-        <f t="shared" si="0"/>
+      <c r="P10" s="3">
+        <f>P9 + J10 - (H10 + K10+ L10 + M10)</f>
         <v>1.1866666666667243</v>
       </c>
-      <c r="P10" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q10" s="4">
+        <f>Q9 + H10 - K10</f>
         <v>1.5933333333333053</v>
       </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="2"/>
+      <c r="R10" s="1">
+        <f>R9 + H10 - L10</f>
         <v>-0.40666666666669471</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -743,41 +757,41 @@
         <v>88.33</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>80.03</v>
       </c>
       <c r="F11" s="2">
         <v>59.99</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1265.02</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>421.67333333333335</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1265.02</v>
       </c>
       <c r="L11" s="1">
         <v>421.67</v>
       </c>
-      <c r="O11" s="3">
-        <f t="shared" si="0"/>
+      <c r="P11" s="3">
+        <f>P10 + J11 - (H11 + K11+ L11 + M11)</f>
         <v>422.86333333333334</v>
       </c>
-      <c r="P11" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q11" s="4">
+        <f>Q10 + H11 - K11</f>
         <v>423.26666666666665</v>
       </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="2"/>
+      <c r="R11" s="1">
+        <f>R10 + H11 - L11</f>
         <v>-0.40333333333336441</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -788,38 +802,38 @@
         <v>101.95</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>88.33</v>
       </c>
       <c r="F12" s="2">
         <v>59.99</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1273.32</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>424.44</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1273.32</v>
       </c>
-      <c r="O12" s="3">
-        <f t="shared" si="0"/>
+      <c r="P12" s="3">
+        <f>P11 + J12 - (H12 + K12+ L12 + M12)</f>
         <v>1271.7433333333333</v>
       </c>
-      <c r="P12" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q12" s="4">
+        <f>Q11 + H12 - K12</f>
         <v>847.70666666666671</v>
       </c>
-      <c r="Q12" s="1">
-        <f t="shared" si="2"/>
+      <c r="R12" s="1">
+        <f>R11 + H12 - L12</f>
         <v>424.03666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -830,22 +844,22 @@
         <v>135.81</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>101.95</v>
       </c>
       <c r="F13" s="2">
         <v>59.99</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1286.94</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>428.98</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1286.94</v>
       </c>
       <c r="K13" s="4">
@@ -854,20 +868,20 @@
       <c r="L13" s="1">
         <v>854</v>
       </c>
-      <c r="O13" s="3">
-        <f t="shared" si="0"/>
+      <c r="P13" s="3">
+        <f>P12 + J13 - (H13 + K13+ L13 + M13)</f>
         <v>425.70333333333338</v>
       </c>
-      <c r="P13" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q13" s="4">
+        <f>Q12 + H13 - K13</f>
         <v>426.68666666666672</v>
       </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="2"/>
+      <c r="R13" s="1">
+        <f>R12 + H13 - L13</f>
         <v>-0.98333333333334849</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2017</v>
       </c>
@@ -881,38 +895,38 @@
         <v>191.54</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>135.81</v>
       </c>
       <c r="F14" s="2">
         <v>59.99</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1320.8</v>
       </c>
       <c r="H14" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>440.26666666666665</v>
       </c>
       <c r="J14" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1320.8</v>
       </c>
-      <c r="O14" s="3">
-        <f t="shared" si="0"/>
+      <c r="P14" s="3">
+        <f>P13 + J14 - (H14 + K14+ L14 + M14)</f>
         <v>1306.2366666666667</v>
       </c>
-      <c r="P14" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q14" s="4">
+        <f>Q13 + H14 - K14</f>
         <v>866.95333333333338</v>
       </c>
-      <c r="Q14" s="1">
-        <f t="shared" si="2"/>
+      <c r="R14" s="1">
+        <f>R13 + H14 - L14</f>
         <v>439.2833333333333</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -923,22 +937,22 @@
         <v>214.48</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>191.54</v>
       </c>
       <c r="F15" s="2">
         <v>59.99</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1376.53</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>458.84333333333331</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1376.53</v>
       </c>
       <c r="K15" s="4">
@@ -947,20 +961,20 @@
       <c r="L15" s="1">
         <v>899.11</v>
       </c>
-      <c r="O15" s="3">
-        <f t="shared" si="0"/>
+      <c r="P15" s="3">
+        <f>P14 + J15 - (H15 + K15+ L15 + M15)</f>
         <v>-3.1866666666669516</v>
       </c>
-      <c r="P15" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q15" s="4">
+        <f>Q14 + H15 - K15</f>
         <v>-2.2033333333333758</v>
       </c>
-      <c r="Q15" s="1">
-        <f t="shared" si="2"/>
+      <c r="R15" s="1">
+        <f>R14 + H15 - L15</f>
         <v>-0.98333333333346218</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -971,22 +985,22 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>214.48</v>
       </c>
       <c r="F16" s="2">
         <v>59.99</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1399.47</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>466.49</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1399.47</v>
       </c>
       <c r="K16" s="4">
@@ -995,20 +1009,20 @@
       <c r="L16" s="1">
         <v>466.5</v>
       </c>
-      <c r="O16" s="3">
-        <f t="shared" si="0"/>
+      <c r="P16" s="3">
+        <f>P15 + J16 - (H16 + K16+ L16 + M16)</f>
         <v>-3.2066666666669335</v>
       </c>
-      <c r="P16" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q16" s="4">
+        <f>Q15 + H16 - K16</f>
         <v>-2.2133333333333667</v>
       </c>
-      <c r="Q16" s="1">
-        <f t="shared" si="2"/>
+      <c r="R16" s="1">
+        <f>R15 + H16 - L16</f>
         <v>-0.99333333333345308</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1019,38 +1033,38 @@
         <v>271.08999999999997</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17" s="2">
         <v>59.99</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1184.99</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>394.99666666666667</v>
       </c>
       <c r="J17" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1184.99</v>
       </c>
-      <c r="O17" s="3">
-        <f t="shared" si="0"/>
+      <c r="P17" s="3">
+        <f>P16 + J17 - (H17 + K17+ L17 + M17)</f>
         <v>786.78666666666641</v>
       </c>
-      <c r="P17" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q17" s="4">
+        <f>Q16 + H17 - K17</f>
         <v>392.7833333333333</v>
       </c>
-      <c r="Q17" s="1">
-        <f t="shared" si="2"/>
+      <c r="R17" s="1">
+        <f>R16 + H17 - L17</f>
         <v>394.00333333333322</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>4</v>
       </c>
@@ -1061,41 +1075,41 @@
         <v>116.12</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>271.08999999999997</v>
       </c>
       <c r="F18" s="2">
         <v>59.99</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1456.08</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>485.35999999999996</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1456.08</v>
       </c>
       <c r="L18" s="1">
         <v>880.36</v>
       </c>
-      <c r="O18" s="3">
-        <f t="shared" si="0"/>
+      <c r="P18" s="3">
+        <f>P17 + J18 - (H18 + K18+ L18 + M18)</f>
         <v>877.14666666666631</v>
       </c>
-      <c r="P18" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q18" s="4">
+        <f>Q17 + H18 - K18</f>
         <v>878.1433333333332</v>
       </c>
-      <c r="Q18" s="1">
-        <f t="shared" si="2"/>
+      <c r="R18" s="1">
+        <f>R17 + H18 - L18</f>
         <v>-0.99666666666678339</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>5</v>
       </c>
@@ -1106,38 +1120,38 @@
         <v>106.96</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>116.12</v>
       </c>
       <c r="F19" s="2">
         <v>59.99</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1301.1099999999999</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>433.70333333333332</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1301.1099999999999</v>
       </c>
-      <c r="O19" s="3">
-        <f t="shared" si="0"/>
+      <c r="P19" s="3">
+        <f>P18 + J19 - (H19 + K19+ L19 + M19)</f>
         <v>1744.5533333333328</v>
       </c>
-      <c r="P19" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q19" s="4">
+        <f>Q18 + H19 - K19</f>
         <v>1311.8466666666666</v>
       </c>
-      <c r="R19" s="5">
-        <f t="shared" ref="R19:R26" si="7">R18 + H19 - M19</f>
+      <c r="S19" s="5">
+        <f>S18 + H19 - M19</f>
         <v>433.70333333333332</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -1148,22 +1162,22 @@
         <v>72</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>106.96</v>
       </c>
       <c r="F20" s="2">
         <v>59.99</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1291.95</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>430.65000000000003</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1291.95</v>
       </c>
       <c r="K20" s="4">
@@ -1172,20 +1186,20 @@
       <c r="M20" s="5">
         <v>864.36</v>
       </c>
-      <c r="O20" s="3">
-        <f t="shared" si="0"/>
+      <c r="P20" s="3">
+        <f>P19 + J20 - (H20 + K20+ L20 + M20)</f>
         <v>417.43333333333294</v>
       </c>
-      <c r="P20" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q20" s="4">
+        <f>Q19 + H20 - K20</f>
         <v>418.43666666666672</v>
       </c>
-      <c r="R20" s="5">
-        <f t="shared" si="7"/>
+      <c r="S20" s="5">
+        <f>S19 + H20 - M20</f>
         <v>-6.6666666666606034E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -1196,38 +1210,38 @@
         <v>72.37</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="F21" s="2">
         <v>59.99</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1256.99</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>418.99666666666667</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1256.99</v>
       </c>
-      <c r="O21" s="3">
-        <f t="shared" si="0"/>
+      <c r="P21" s="3">
+        <f>P20 + J21 - (H21 + K21+ L21 + M21)</f>
         <v>1255.4266666666663</v>
       </c>
-      <c r="P21" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q21" s="4">
+        <f>Q20 + H21 - K21</f>
         <v>837.43333333333339</v>
       </c>
-      <c r="R21" s="5">
-        <f t="shared" si="7"/>
+      <c r="S21" s="5">
+        <f>S20 + H21 - M21</f>
         <v>418.99</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -1238,22 +1252,22 @@
         <v>71.7</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>72.37</v>
       </c>
       <c r="F22" s="2">
         <v>59.99</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1277.3599999999999</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>425.78666666666663</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1277.3599999999999</v>
       </c>
       <c r="K22" s="4">
@@ -1262,20 +1276,20 @@
       <c r="M22" s="5">
         <v>844.79</v>
       </c>
-      <c r="O22" s="3">
-        <f t="shared" si="0"/>
+      <c r="P22" s="3">
+        <f>P21 + J22 - (H22 + K22+ L22 + M22)</f>
         <v>-337.79000000000087</v>
       </c>
-      <c r="P22" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q22" s="4">
+        <f>Q21 + H22 - K22</f>
         <v>-336.78</v>
       </c>
-      <c r="R22" s="5">
-        <f t="shared" si="7"/>
+      <c r="S22" s="5">
+        <f>S21 + H22 - M22</f>
         <v>-1.3333333333321207E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -1286,38 +1300,38 @@
         <v>79.25</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>71.7</v>
       </c>
       <c r="F23" s="2">
         <v>59.99</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1276.69</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>425.56333333333333</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1276.69</v>
       </c>
-      <c r="O23" s="3">
-        <f t="shared" si="0"/>
+      <c r="P23" s="3">
+        <f>P22 + J23 - (H23 + K23+ L23 + M23)</f>
         <v>513.33666666666591</v>
       </c>
-      <c r="P23" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q23" s="4">
+        <f>Q22 + H23 - K23</f>
         <v>88.78333333333336</v>
       </c>
-      <c r="R23" s="5">
-        <f t="shared" si="7"/>
+      <c r="S23" s="5">
+        <f>S22 + H23 - M23</f>
         <v>425.55</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>10</v>
       </c>
@@ -1328,41 +1342,41 @@
         <v>135.03</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>79.25</v>
       </c>
       <c r="F24" s="2">
         <v>59.99</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1284.24</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>428.08</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1284.24</v>
       </c>
       <c r="M24" s="5">
         <v>911</v>
       </c>
-      <c r="O24" s="3">
-        <f t="shared" si="0"/>
+      <c r="P24" s="3">
+        <f>P23 + J24 - (H24 + K24+ L24 + M24)</f>
         <v>458.49666666666599</v>
       </c>
-      <c r="P24" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q24" s="4">
+        <f>Q23 + H24 - K24</f>
         <v>516.86333333333334</v>
       </c>
-      <c r="R24" s="5">
-        <f t="shared" si="7"/>
+      <c r="S24" s="5">
+        <f>S23 + H24 - M24</f>
         <v>-57.370000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -1373,38 +1387,38 @@
         <v>158.99</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>135.03</v>
       </c>
       <c r="F25" s="2">
         <v>59.99</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1340.02</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>446.67333333333335</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1340.02</v>
       </c>
-      <c r="O25" s="3">
-        <f t="shared" si="0"/>
+      <c r="P25" s="3">
+        <f>P24 + J25 - (H25 + K25+ L25 + M25)</f>
         <v>1351.8433333333326</v>
       </c>
-      <c r="P25" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q25" s="4">
+        <f>Q24 + H25 - K25</f>
         <v>963.53666666666663</v>
       </c>
-      <c r="R25" s="5">
-        <f t="shared" si="7"/>
+      <c r="S25" s="5">
+        <f>S24 + H25 - M25</f>
         <v>389.30333333333334</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2018</v>
       </c>
@@ -1418,41 +1432,41 @@
         <v>150.13999999999999</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>158.99</v>
       </c>
       <c r="F26" s="2">
         <v>59.99</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1363.98</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>454.66</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1363.98</v>
       </c>
       <c r="K26" s="4">
         <v>1100</v>
       </c>
-      <c r="O26" s="3">
-        <f t="shared" si="0"/>
+      <c r="P26" s="3">
+        <f>P25 + J26 - (H26 + K26+ L26 + M26)</f>
         <v>1161.1633333333327</v>
       </c>
-      <c r="P26" s="4">
-        <f t="shared" si="1"/>
+      <c r="Q26" s="4">
+        <f>Q25 + H26 - K26</f>
         <v>318.19666666666672</v>
       </c>
-      <c r="R26" s="5">
-        <f t="shared" si="7"/>
+      <c r="S26" s="5">
+        <f>S25 + H26 - M26</f>
         <v>843.96333333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -1463,41 +1477,41 @@
         <v>157.99</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>150.13999999999999</v>
       </c>
       <c r="F27" s="2">
         <v>59.99</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1355.1299999999999</v>
       </c>
       <c r="H27" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>451.71</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1355.1299999999999</v>
       </c>
       <c r="M27" s="5">
         <v>500</v>
       </c>
-      <c r="O27" s="3">
-        <f t="shared" ref="O27:O28" si="8">O26 + J27 - (H27 + K27+ L27 + M27)</f>
+      <c r="P27" s="3">
+        <f>P26 + J27 - (H27 + K27+ L27 + M27)</f>
         <v>1564.5833333333326</v>
       </c>
-      <c r="P27" s="4">
-        <f t="shared" ref="P27:P30" si="9">P26 + H27 - K27</f>
+      <c r="Q27" s="4">
+        <f>Q26 + H27 - K27</f>
         <v>769.90666666666675</v>
       </c>
-      <c r="R27" s="5">
-        <f t="shared" ref="R27:R30" si="10">R26 + H27 - M27</f>
+      <c r="S27" s="5">
+        <f>S26 + H27 - M27</f>
         <v>795.6733333333334</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -1508,22 +1522,22 @@
         <v>177.54</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>157.99</v>
       </c>
       <c r="F28" s="2">
         <v>59.99</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1362.98</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>454.32666666666665</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1362.98</v>
       </c>
       <c r="K28" s="4">
@@ -1532,23 +1546,23 @@
       <c r="M28" s="5">
         <v>1170</v>
       </c>
-      <c r="O28" s="3">
-        <f t="shared" si="8"/>
+      <c r="P28" s="3">
+        <f>P27 + J28 - (H28 + K28+ L28 + M28)</f>
         <v>-496.76333333333423</v>
       </c>
-      <c r="P28" s="4">
-        <f t="shared" si="9"/>
+      <c r="Q28" s="4">
+        <f>Q27 + H28 - K28</f>
         <v>-575.76666666666665</v>
       </c>
-      <c r="R28" s="5">
-        <f t="shared" si="10"/>
+      <c r="S28" s="5">
+        <f>S27 + H28 - M28</f>
         <v>80</v>
       </c>
-      <c r="S28" t="s">
+      <c r="U28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -1559,88 +1573,116 @@
         <v>164.3</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>177.54</v>
       </c>
       <c r="F29" s="2">
         <v>59.99</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1382.53</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>460.84333333333331</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1382.53</v>
       </c>
-      <c r="O29" s="3">
-        <f>O28 + J29 - (H29 + K29+ L29 + M29)</f>
+      <c r="P29" s="3">
+        <f>P28 + J29 - (H29 + K29+ L29 + M29)</f>
         <v>424.92333333333244</v>
       </c>
-      <c r="P29" s="4">
-        <f t="shared" si="9"/>
+      <c r="Q29" s="4">
+        <f>Q28 + H29 - K29</f>
         <v>-114.92333333333335</v>
       </c>
-      <c r="R29" s="5">
-        <f t="shared" si="10"/>
+      <c r="S29" s="5">
+        <f>S28 + H29 - M29</f>
         <v>540.84333333333325</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="2">
         <v>1145</v>
       </c>
+      <c r="D30" s="2">
+        <v>129.44</v>
+      </c>
       <c r="E30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>164.3</v>
       </c>
       <c r="F30" s="2">
         <v>59.99</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1369.29</v>
       </c>
       <c r="H30" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>456.43</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1369.29</v>
       </c>
       <c r="M30" s="5">
         <v>1000</v>
       </c>
-      <c r="O30" s="3">
-        <f>O29 + J30 - (H30 + K30+ L30 + M30)</f>
+      <c r="P30" s="3">
+        <f>P29 + J30 - (H30 + K30+ L30 + M30)</f>
         <v>337.78333333333239</v>
       </c>
-      <c r="P30" s="4">
-        <f t="shared" si="9"/>
+      <c r="Q30" s="4">
+        <f>Q29 + H30 - K30</f>
         <v>341.50666666666666</v>
       </c>
-      <c r="R30" s="5">
-        <f t="shared" si="10"/>
+      <c r="S30" s="5">
+        <f>S29 + H30 - M30</f>
         <v>-2.7266666666666879</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="2">
         <v>1145</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>129.44</v>
+      </c>
+      <c r="F31" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>1334.43</v>
+      </c>
+      <c r="H31" s="6">
+        <f t="shared" si="2"/>
+        <v>444.81</v>
+      </c>
+      <c r="N31" s="3">
+        <v>444.81</v>
+      </c>
+      <c r="T31" s="3">
+        <f>T30 + H31 - N31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updated to reflect payments up until July 8th 2018
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -523,10 +523,10 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
+      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,15 +686,15 @@
         <v>422</v>
       </c>
       <c r="P9" s="3">
-        <f>P8 + J9 - (H9 + K9+ L9 + M9)</f>
+        <f t="shared" ref="P9:P32" si="0">P8 + J9 - (H9 + K9+ L9 + M9)</f>
         <v>1.0199999999999818</v>
       </c>
       <c r="Q9" s="4">
-        <f>Q8 + H9 - K9</f>
+        <f t="shared" ref="Q9:Q30" si="1">Q8 + H9 - K9</f>
         <v>1.5099999999999909</v>
       </c>
       <c r="R9" s="1">
-        <f>R8 + H9 - L9</f>
+        <f t="shared" ref="R9:R18" si="2">R8 + H9 - L9</f>
         <v>-0.49000000000000909</v>
       </c>
     </row>
@@ -709,22 +709,22 @@
         <v>80.03</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" ref="E10:E31" si="0">D9</f>
+        <f t="shared" ref="E10:E32" si="3">D9</f>
         <v>87.26</v>
       </c>
       <c r="F10" s="2">
         <v>59.99</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G31" si="1">C10+E10+F10</f>
+        <f t="shared" ref="G10:G32" si="4">C10+E10+F10</f>
         <v>1272.25</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10:H31" si="2">G10/3</f>
+        <f t="shared" ref="H10:H33" si="5">G10/3</f>
         <v>424.08333333333331</v>
       </c>
       <c r="J10" s="3">
-        <f t="shared" ref="J10:J30" si="3">G10</f>
+        <f t="shared" ref="J10:J32" si="6">G10</f>
         <v>1272.25</v>
       </c>
       <c r="K10" s="4">
@@ -734,15 +734,15 @@
         <v>424</v>
       </c>
       <c r="P10" s="3">
-        <f>P9 + J10 - (H10 + K10+ L10 + M10)</f>
+        <f t="shared" si="0"/>
         <v>1.1866666666667243</v>
       </c>
       <c r="Q10" s="4">
-        <f>Q9 + H10 - K10</f>
+        <f t="shared" si="1"/>
         <v>1.5933333333333053</v>
       </c>
       <c r="R10" s="1">
-        <f>R9 + H10 - L10</f>
+        <f t="shared" si="2"/>
         <v>-0.40666666666669471</v>
       </c>
     </row>
@@ -757,37 +757,37 @@
         <v>88.33</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>80.03</v>
       </c>
       <c r="F11" s="2">
         <v>59.99</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1265.02</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>421.67333333333335</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1265.02</v>
       </c>
       <c r="L11" s="1">
         <v>421.67</v>
       </c>
       <c r="P11" s="3">
-        <f>P10 + J11 - (H11 + K11+ L11 + M11)</f>
+        <f t="shared" si="0"/>
         <v>422.86333333333334</v>
       </c>
       <c r="Q11" s="4">
-        <f>Q10 + H11 - K11</f>
+        <f t="shared" si="1"/>
         <v>423.26666666666665</v>
       </c>
       <c r="R11" s="1">
-        <f>R10 + H11 - L11</f>
+        <f t="shared" si="2"/>
         <v>-0.40333333333336441</v>
       </c>
     </row>
@@ -802,34 +802,34 @@
         <v>101.95</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>88.33</v>
       </c>
       <c r="F12" s="2">
         <v>59.99</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1273.32</v>
       </c>
       <c r="H12" s="6">
+        <f t="shared" si="5"/>
+        <v>424.44</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="6"/>
+        <v>1273.32</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" si="0"/>
+        <v>1271.7433333333333</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="1"/>
+        <v>847.70666666666671</v>
+      </c>
+      <c r="R12" s="1">
         <f t="shared" si="2"/>
-        <v>424.44</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="3"/>
-        <v>1273.32</v>
-      </c>
-      <c r="P12" s="3">
-        <f>P11 + J12 - (H12 + K12+ L12 + M12)</f>
-        <v>1271.7433333333333</v>
-      </c>
-      <c r="Q12" s="4">
-        <f>Q11 + H12 - K12</f>
-        <v>847.70666666666671</v>
-      </c>
-      <c r="R12" s="1">
-        <f>R11 + H12 - L12</f>
         <v>424.03666666666663</v>
       </c>
     </row>
@@ -844,22 +844,22 @@
         <v>135.81</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>101.95</v>
       </c>
       <c r="F13" s="2">
         <v>59.99</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1286.94</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>428.98</v>
       </c>
       <c r="J13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1286.94</v>
       </c>
       <c r="K13" s="4">
@@ -869,15 +869,15 @@
         <v>854</v>
       </c>
       <c r="P13" s="3">
-        <f>P12 + J13 - (H13 + K13+ L13 + M13)</f>
+        <f t="shared" si="0"/>
         <v>425.70333333333338</v>
       </c>
       <c r="Q13" s="4">
-        <f>Q12 + H13 - K13</f>
+        <f t="shared" si="1"/>
         <v>426.68666666666672</v>
       </c>
       <c r="R13" s="1">
-        <f>R12 + H13 - L13</f>
+        <f t="shared" si="2"/>
         <v>-0.98333333333334849</v>
       </c>
     </row>
@@ -895,34 +895,34 @@
         <v>191.54</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>135.81</v>
       </c>
       <c r="F14" s="2">
         <v>59.99</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1320.8</v>
       </c>
       <c r="H14" s="6">
+        <f t="shared" si="5"/>
+        <v>440.26666666666665</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="6"/>
+        <v>1320.8</v>
+      </c>
+      <c r="P14" s="3">
+        <f t="shared" si="0"/>
+        <v>1306.2366666666667</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="1"/>
+        <v>866.95333333333338</v>
+      </c>
+      <c r="R14" s="1">
         <f t="shared" si="2"/>
-        <v>440.26666666666665</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="3"/>
-        <v>1320.8</v>
-      </c>
-      <c r="P14" s="3">
-        <f>P13 + J14 - (H14 + K14+ L14 + M14)</f>
-        <v>1306.2366666666667</v>
-      </c>
-      <c r="Q14" s="4">
-        <f>Q13 + H14 - K14</f>
-        <v>866.95333333333338</v>
-      </c>
-      <c r="R14" s="1">
-        <f>R13 + H14 - L14</f>
         <v>439.2833333333333</v>
       </c>
     </row>
@@ -937,22 +937,22 @@
         <v>214.48</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>191.54</v>
       </c>
       <c r="F15" s="2">
         <v>59.99</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1376.53</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>458.84333333333331</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1376.53</v>
       </c>
       <c r="K15" s="4">
@@ -962,15 +962,15 @@
         <v>899.11</v>
       </c>
       <c r="P15" s="3">
-        <f>P14 + J15 - (H15 + K15+ L15 + M15)</f>
+        <f t="shared" si="0"/>
         <v>-3.1866666666669516</v>
       </c>
       <c r="Q15" s="4">
-        <f>Q14 + H15 - K15</f>
+        <f t="shared" si="1"/>
         <v>-2.2033333333333758</v>
       </c>
       <c r="R15" s="1">
-        <f>R14 + H15 - L15</f>
+        <f t="shared" si="2"/>
         <v>-0.98333333333346218</v>
       </c>
     </row>
@@ -985,22 +985,22 @@
         <v>0</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>214.48</v>
       </c>
       <c r="F16" s="2">
         <v>59.99</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1399.47</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>466.49</v>
       </c>
       <c r="J16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1399.47</v>
       </c>
       <c r="K16" s="4">
@@ -1010,15 +1010,15 @@
         <v>466.5</v>
       </c>
       <c r="P16" s="3">
-        <f>P15 + J16 - (H16 + K16+ L16 + M16)</f>
+        <f t="shared" si="0"/>
         <v>-3.2066666666669335</v>
       </c>
       <c r="Q16" s="4">
-        <f>Q15 + H16 - K16</f>
+        <f t="shared" si="1"/>
         <v>-2.2133333333333667</v>
       </c>
       <c r="R16" s="1">
-        <f>R15 + H16 - L16</f>
+        <f t="shared" si="2"/>
         <v>-0.99333333333345308</v>
       </c>
     </row>
@@ -1033,34 +1033,34 @@
         <v>271.08999999999997</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F17" s="2">
         <v>59.99</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1184.99</v>
       </c>
       <c r="H17" s="6">
+        <f t="shared" si="5"/>
+        <v>394.99666666666667</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="6"/>
+        <v>1184.99</v>
+      </c>
+      <c r="P17" s="3">
+        <f t="shared" si="0"/>
+        <v>786.78666666666641</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="1"/>
+        <v>392.7833333333333</v>
+      </c>
+      <c r="R17" s="1">
         <f t="shared" si="2"/>
-        <v>394.99666666666667</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" si="3"/>
-        <v>1184.99</v>
-      </c>
-      <c r="P17" s="3">
-        <f>P16 + J17 - (H17 + K17+ L17 + M17)</f>
-        <v>786.78666666666641</v>
-      </c>
-      <c r="Q17" s="4">
-        <f>Q16 + H17 - K17</f>
-        <v>392.7833333333333</v>
-      </c>
-      <c r="R17" s="1">
-        <f>R16 + H17 - L17</f>
         <v>394.00333333333322</v>
       </c>
     </row>
@@ -1075,37 +1075,37 @@
         <v>116.12</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>271.08999999999997</v>
       </c>
       <c r="F18" s="2">
         <v>59.99</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1456.08</v>
       </c>
       <c r="H18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>485.35999999999996</v>
       </c>
       <c r="J18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1456.08</v>
       </c>
       <c r="L18" s="1">
         <v>880.36</v>
       </c>
       <c r="P18" s="3">
-        <f>P17 + J18 - (H18 + K18+ L18 + M18)</f>
+        <f t="shared" si="0"/>
         <v>877.14666666666631</v>
       </c>
       <c r="Q18" s="4">
-        <f>Q17 + H18 - K18</f>
+        <f t="shared" si="1"/>
         <v>878.1433333333332</v>
       </c>
       <c r="R18" s="1">
-        <f>R17 + H18 - L18</f>
+        <f t="shared" si="2"/>
         <v>-0.99666666666678339</v>
       </c>
     </row>
@@ -1120,34 +1120,34 @@
         <v>106.96</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>116.12</v>
       </c>
       <c r="F19" s="2">
         <v>59.99</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1301.1099999999999</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>433.70333333333332</v>
       </c>
       <c r="J19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1301.1099999999999</v>
       </c>
       <c r="P19" s="3">
-        <f>P18 + J19 - (H19 + K19+ L19 + M19)</f>
+        <f t="shared" si="0"/>
         <v>1744.5533333333328</v>
       </c>
       <c r="Q19" s="4">
-        <f>Q18 + H19 - K19</f>
+        <f t="shared" si="1"/>
         <v>1311.8466666666666</v>
       </c>
       <c r="S19" s="5">
-        <f>S18 + H19 - M19</f>
+        <f t="shared" ref="S19:S32" si="7">S18 + H19 - M19</f>
         <v>433.70333333333332</v>
       </c>
     </row>
@@ -1162,22 +1162,22 @@
         <v>72</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>106.96</v>
       </c>
       <c r="F20" s="2">
         <v>59.99</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1291.95</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>430.65000000000003</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1291.95</v>
       </c>
       <c r="K20" s="4">
@@ -1187,15 +1187,15 @@
         <v>864.36</v>
       </c>
       <c r="P20" s="3">
-        <f>P19 + J20 - (H20 + K20+ L20 + M20)</f>
+        <f t="shared" si="0"/>
         <v>417.43333333333294</v>
       </c>
       <c r="Q20" s="4">
-        <f>Q19 + H20 - K20</f>
+        <f t="shared" si="1"/>
         <v>418.43666666666672</v>
       </c>
       <c r="S20" s="5">
-        <f>S19 + H20 - M20</f>
+        <f t="shared" si="7"/>
         <v>-6.6666666666606034E-3</v>
       </c>
     </row>
@@ -1210,34 +1210,34 @@
         <v>72.37</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="F21" s="2">
         <v>59.99</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1256.99</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>418.99666666666667</v>
       </c>
       <c r="J21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1256.99</v>
       </c>
       <c r="P21" s="3">
-        <f>P20 + J21 - (H21 + K21+ L21 + M21)</f>
+        <f t="shared" si="0"/>
         <v>1255.4266666666663</v>
       </c>
       <c r="Q21" s="4">
-        <f>Q20 + H21 - K21</f>
+        <f t="shared" si="1"/>
         <v>837.43333333333339</v>
       </c>
       <c r="S21" s="5">
-        <f>S20 + H21 - M21</f>
+        <f t="shared" si="7"/>
         <v>418.99</v>
       </c>
     </row>
@@ -1252,22 +1252,22 @@
         <v>71.7</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>72.37</v>
       </c>
       <c r="F22" s="2">
         <v>59.99</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1277.3599999999999</v>
       </c>
       <c r="H22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>425.78666666666663</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1277.3599999999999</v>
       </c>
       <c r="K22" s="4">
@@ -1277,15 +1277,15 @@
         <v>844.79</v>
       </c>
       <c r="P22" s="3">
-        <f>P21 + J22 - (H22 + K22+ L22 + M22)</f>
+        <f t="shared" si="0"/>
         <v>-337.79000000000087</v>
       </c>
       <c r="Q22" s="4">
-        <f>Q21 + H22 - K22</f>
+        <f t="shared" si="1"/>
         <v>-336.78</v>
       </c>
       <c r="S22" s="5">
-        <f>S21 + H22 - M22</f>
+        <f t="shared" si="7"/>
         <v>-1.3333333333321207E-2</v>
       </c>
     </row>
@@ -1300,34 +1300,34 @@
         <v>79.25</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>71.7</v>
       </c>
       <c r="F23" s="2">
         <v>59.99</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1276.69</v>
       </c>
       <c r="H23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>425.56333333333333</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1276.69</v>
       </c>
       <c r="P23" s="3">
-        <f>P22 + J23 - (H23 + K23+ L23 + M23)</f>
+        <f t="shared" si="0"/>
         <v>513.33666666666591</v>
       </c>
       <c r="Q23" s="4">
-        <f>Q22 + H23 - K23</f>
+        <f t="shared" si="1"/>
         <v>88.78333333333336</v>
       </c>
       <c r="S23" s="5">
-        <f>S22 + H23 - M23</f>
+        <f t="shared" si="7"/>
         <v>425.55</v>
       </c>
     </row>
@@ -1342,37 +1342,37 @@
         <v>135.03</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>79.25</v>
       </c>
       <c r="F24" s="2">
         <v>59.99</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1284.24</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>428.08</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1284.24</v>
       </c>
       <c r="M24" s="5">
         <v>911</v>
       </c>
       <c r="P24" s="3">
-        <f>P23 + J24 - (H24 + K24+ L24 + M24)</f>
+        <f t="shared" si="0"/>
         <v>458.49666666666599</v>
       </c>
       <c r="Q24" s="4">
-        <f>Q23 + H24 - K24</f>
+        <f t="shared" si="1"/>
         <v>516.86333333333334</v>
       </c>
       <c r="S24" s="5">
-        <f>S23 + H24 - M24</f>
+        <f t="shared" si="7"/>
         <v>-57.370000000000005</v>
       </c>
     </row>
@@ -1387,34 +1387,34 @@
         <v>158.99</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>135.03</v>
       </c>
       <c r="F25" s="2">
         <v>59.99</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1340.02</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>446.67333333333335</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1340.02</v>
       </c>
       <c r="P25" s="3">
-        <f>P24 + J25 - (H25 + K25+ L25 + M25)</f>
+        <f t="shared" si="0"/>
         <v>1351.8433333333326</v>
       </c>
       <c r="Q25" s="4">
-        <f>Q24 + H25 - K25</f>
+        <f t="shared" si="1"/>
         <v>963.53666666666663</v>
       </c>
       <c r="S25" s="5">
-        <f>S24 + H25 - M25</f>
+        <f t="shared" si="7"/>
         <v>389.30333333333334</v>
       </c>
     </row>
@@ -1432,37 +1432,37 @@
         <v>150.13999999999999</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>158.99</v>
       </c>
       <c r="F26" s="2">
         <v>59.99</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1363.98</v>
       </c>
       <c r="H26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>454.66</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1363.98</v>
       </c>
       <c r="K26" s="4">
         <v>1100</v>
       </c>
       <c r="P26" s="3">
-        <f>P25 + J26 - (H26 + K26+ L26 + M26)</f>
+        <f t="shared" si="0"/>
         <v>1161.1633333333327</v>
       </c>
       <c r="Q26" s="4">
-        <f>Q25 + H26 - K26</f>
+        <f t="shared" si="1"/>
         <v>318.19666666666672</v>
       </c>
       <c r="S26" s="5">
-        <f>S25 + H26 - M26</f>
+        <f t="shared" si="7"/>
         <v>843.96333333333337</v>
       </c>
     </row>
@@ -1477,37 +1477,37 @@
         <v>157.99</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>150.13999999999999</v>
       </c>
       <c r="F27" s="2">
         <v>59.99</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1355.1299999999999</v>
       </c>
       <c r="H27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>451.71</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1355.1299999999999</v>
       </c>
       <c r="M27" s="5">
         <v>500</v>
       </c>
       <c r="P27" s="3">
-        <f>P26 + J27 - (H27 + K27+ L27 + M27)</f>
+        <f t="shared" si="0"/>
         <v>1564.5833333333326</v>
       </c>
       <c r="Q27" s="4">
-        <f>Q26 + H27 - K27</f>
+        <f t="shared" si="1"/>
         <v>769.90666666666675</v>
       </c>
       <c r="S27" s="5">
-        <f>S26 + H27 - M27</f>
+        <f t="shared" si="7"/>
         <v>795.6733333333334</v>
       </c>
     </row>
@@ -1522,22 +1522,22 @@
         <v>177.54</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>157.99</v>
       </c>
       <c r="F28" s="2">
         <v>59.99</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1362.98</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>454.32666666666665</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1362.98</v>
       </c>
       <c r="K28" s="4">
@@ -1547,15 +1547,15 @@
         <v>1170</v>
       </c>
       <c r="P28" s="3">
-        <f>P27 + J28 - (H28 + K28+ L28 + M28)</f>
+        <f t="shared" si="0"/>
         <v>-496.76333333333423</v>
       </c>
       <c r="Q28" s="4">
-        <f>Q27 + H28 - K28</f>
+        <f t="shared" si="1"/>
         <v>-575.76666666666665</v>
       </c>
       <c r="S28" s="5">
-        <f>S27 + H28 - M28</f>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="U28" t="s">
@@ -1573,34 +1573,34 @@
         <v>164.3</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>177.54</v>
       </c>
       <c r="F29" s="2">
         <v>59.99</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1382.53</v>
       </c>
       <c r="H29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>460.84333333333331</v>
       </c>
       <c r="J29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1382.53</v>
       </c>
       <c r="P29" s="3">
-        <f>P28 + J29 - (H29 + K29+ L29 + M29)</f>
+        <f t="shared" si="0"/>
         <v>424.92333333333244</v>
       </c>
       <c r="Q29" s="4">
-        <f>Q28 + H29 - K29</f>
+        <f t="shared" si="1"/>
         <v>-114.92333333333335</v>
       </c>
       <c r="S29" s="5">
-        <f>S28 + H29 - M29</f>
+        <f t="shared" si="7"/>
         <v>540.84333333333325</v>
       </c>
     </row>
@@ -1615,37 +1615,37 @@
         <v>129.44</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>164.3</v>
       </c>
       <c r="F30" s="2">
         <v>59.99</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1369.29</v>
       </c>
       <c r="H30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>456.43</v>
       </c>
       <c r="J30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1369.29</v>
       </c>
       <c r="M30" s="5">
         <v>1000</v>
       </c>
       <c r="P30" s="3">
-        <f>P29 + J30 - (H30 + K30+ L30 + M30)</f>
+        <f t="shared" si="0"/>
         <v>337.78333333333239</v>
       </c>
       <c r="Q30" s="4">
-        <f>Q29 + H30 - K30</f>
+        <f t="shared" si="1"/>
         <v>341.50666666666666</v>
       </c>
       <c r="S30" s="5">
-        <f>S29 + H30 - M30</f>
+        <f t="shared" si="7"/>
         <v>-2.7266666666666879</v>
       </c>
       <c r="T30" s="3">
@@ -1659,23 +1659,41 @@
       <c r="C31" s="2">
         <v>1145</v>
       </c>
+      <c r="D31" s="2">
+        <v>102.17</v>
+      </c>
       <c r="E31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>129.44</v>
       </c>
       <c r="F31" s="2">
         <v>59.99</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1334.43</v>
       </c>
       <c r="H31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
+        <v>444.81</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="6"/>
+        <v>1334.43</v>
+      </c>
+      <c r="M31" s="5">
         <v>444.81</v>
       </c>
       <c r="N31" s="3">
         <v>444.81</v>
+      </c>
+      <c r="P31" s="3">
+        <f t="shared" si="0"/>
+        <v>782.59333333333245</v>
+      </c>
+      <c r="S31" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.7266666666666879</v>
       </c>
       <c r="T31" s="3">
         <f>T30 + H31 - N31</f>
@@ -1688,6 +1706,40 @@
       </c>
       <c r="C32" s="2">
         <v>1145</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="3"/>
+        <v>102.17</v>
+      </c>
+      <c r="F32" s="2">
+        <v>59.99</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="4"/>
+        <v>1307.1600000000001</v>
+      </c>
+      <c r="H32" s="6">
+        <f t="shared" si="5"/>
+        <v>435.72</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="6"/>
+        <v>1307.1600000000001</v>
+      </c>
+      <c r="N32" s="3">
+        <v>400</v>
+      </c>
+      <c r="P32" s="3">
+        <f t="shared" si="0"/>
+        <v>1654.0333333333326</v>
+      </c>
+      <c r="S32" s="5">
+        <f t="shared" si="7"/>
+        <v>432.99333333333334</v>
+      </c>
+      <c r="T32" s="3">
+        <f>T31 + H32 - N32</f>
+        <v>35.720000000000027</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added Nick's pyament for July
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -526,7 +526,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M30" sqref="M30"/>
+      <selection pane="bottomRight" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,7 +720,7 @@
         <v>1272.25</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10:H33" si="5">G10/3</f>
+        <f t="shared" ref="H10:H32" si="5">G10/3</f>
         <v>424.08333333333331</v>
       </c>
       <c r="J10" s="3">
@@ -1726,16 +1726,19 @@
         <f t="shared" si="6"/>
         <v>1307.1600000000001</v>
       </c>
+      <c r="M32" s="5">
+        <v>433</v>
+      </c>
       <c r="N32" s="3">
         <v>400</v>
       </c>
       <c r="P32" s="3">
         <f t="shared" si="0"/>
-        <v>1654.0333333333326</v>
+        <v>1221.0333333333326</v>
       </c>
       <c r="S32" s="5">
         <f t="shared" si="7"/>
-        <v>432.99333333333334</v>
+        <v>-6.6666666666606034E-3</v>
       </c>
       <c r="T32" s="3">
         <f>T31 + H32 - N32</f>

</xml_diff>

<commit_message>
Updating with Onnos payment for April
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royts\Documents\Hayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6BAF7-FAD9-4FDB-9E55-D3D647AC3B6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE53C28-E3D3-49C3-A238-85F4CCF08FEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11680" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -555,10 +555,10 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A40" sqref="A40:XFD40"/>
+      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,26 +756,26 @@
         <v>80.03</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" ref="E10:E41" si="2">D9</f>
+        <f t="shared" ref="E10:E42" si="2">D9</f>
         <v>87.26</v>
       </c>
       <c r="F10" s="1">
         <v>59.99</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" ref="G10:G41" si="3">C10/3</f>
+        <f t="shared" ref="G10:G42" si="3">C10/3</f>
         <v>375</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H41" si="4">(E10+F10)/3</f>
+        <f t="shared" ref="H10:H42" si="4">(E10+F10)/3</f>
         <v>49.083333333333336</v>
       </c>
       <c r="I10" s="3">
-        <f t="shared" ref="I10:I41" si="5">G10+H10</f>
+        <f t="shared" ref="I10:I42" si="5">G10+H10</f>
         <v>424.08333333333331</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" ref="K10:K40" si="6">3 *I10</f>
+        <f t="shared" ref="K10:K42" si="6">3 *I10</f>
         <v>1272.25</v>
       </c>
       <c r="L10" s="5">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="V36" s="8"/>
       <c r="W36" s="11">
-        <f>W35 + I36 - P36</f>
+        <f t="shared" ref="W36:W42" si="9">W35 + I36 - P36</f>
         <v>49.616666666666674</v>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
         <v>486.26</v>
       </c>
       <c r="R37" s="4">
-        <f t="shared" ref="R37:R40" si="9">R36 + K37 - (I37 + L37+ M37 + N37 + O37 + P37)</f>
+        <f t="shared" ref="R37:R42" si="10">R36 + K37 - (I37 + L37+ M37 + N37 + O37 + P37)</f>
         <v>-1719.7466666666674</v>
       </c>
       <c r="S37" s="5">
@@ -2138,7 +2138,7 @@
         <v>-2162.3966666666665</v>
       </c>
       <c r="W37" s="11">
-        <f>W36 + I37 - P37</f>
+        <f t="shared" si="9"/>
         <v>3.3333333333871451E-3</v>
       </c>
     </row>
@@ -2183,15 +2183,15 @@
         <v>445.17</v>
       </c>
       <c r="R38" s="4">
+        <f t="shared" si="10"/>
+        <v>-1274.5766666666673</v>
+      </c>
+      <c r="S38" s="5">
+        <f t="shared" ref="S38:S42" si="11">S37 + I38 - L38</f>
+        <v>-1717.2266666666665</v>
+      </c>
+      <c r="W38" s="11">
         <f t="shared" si="9"/>
-        <v>-1274.5766666666673</v>
-      </c>
-      <c r="S38" s="5">
-        <f t="shared" ref="S38:S43" si="10">S37 + I38 - L38</f>
-        <v>-1717.2266666666665</v>
-      </c>
-      <c r="W38" s="11">
-        <f>W37 + I38 - P38</f>
         <v>3.3333333333871451E-3</v>
       </c>
     </row>
@@ -2233,15 +2233,15 @@
         <v>444.33000000000004</v>
       </c>
       <c r="R39" s="4">
+        <f t="shared" si="10"/>
+        <v>-830.24666666666712</v>
+      </c>
+      <c r="S39" s="5">
+        <f t="shared" si="11"/>
+        <v>-1272.8966666666665</v>
+      </c>
+      <c r="W39" s="11">
         <f t="shared" si="9"/>
-        <v>-830.24666666666712</v>
-      </c>
-      <c r="S39" s="5">
-        <f t="shared" si="10"/>
-        <v>-1272.8966666666665</v>
-      </c>
-      <c r="W39" s="11">
-        <f>W38 + I39 - P39</f>
         <v>3.3333333333871451E-3</v>
       </c>
     </row>
@@ -2283,15 +2283,15 @@
         <v>455.44</v>
       </c>
       <c r="R40" s="4">
+        <f t="shared" si="10"/>
+        <v>-374.81333333333384</v>
+      </c>
+      <c r="S40" s="5">
+        <f t="shared" si="11"/>
+        <v>-817.45999999999981</v>
+      </c>
+      <c r="W40" s="11">
         <f t="shared" si="9"/>
-        <v>-374.81333333333384</v>
-      </c>
-      <c r="S40" s="5">
-        <f t="shared" si="10"/>
-        <v>-817.45999999999981</v>
-      </c>
-      <c r="W40" s="11">
-        <f>W39 + I40 - P40</f>
         <v>0</v>
       </c>
     </row>
@@ -2302,6 +2302,9 @@
       <c r="C41" s="1">
         <v>1145</v>
       </c>
+      <c r="D41" s="1">
+        <v>147.07</v>
+      </c>
       <c r="E41" s="1">
         <f t="shared" si="2"/>
         <v>194.78</v>
@@ -2321,9 +2324,24 @@
         <f t="shared" si="5"/>
         <v>466.59000000000003</v>
       </c>
+      <c r="K41" s="4">
+        <f t="shared" si="6"/>
+        <v>1399.77</v>
+      </c>
+      <c r="L41" s="5">
+        <v>100</v>
+      </c>
+      <c r="R41" s="4">
+        <f t="shared" si="10"/>
+        <v>458.36666666666599</v>
+      </c>
       <c r="S41" s="5">
-        <f t="shared" si="10"/>
-        <v>-350.86999999999978</v>
+        <f t="shared" si="11"/>
+        <v>-450.86999999999978</v>
+      </c>
+      <c r="W41" s="11">
+        <f t="shared" si="9"/>
+        <v>466.59000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.35">
@@ -2333,9 +2351,40 @@
       <c r="C42" s="1">
         <v>1145</v>
       </c>
+      <c r="E42" s="1">
+        <f t="shared" si="2"/>
+        <v>147.07</v>
+      </c>
+      <c r="F42" s="1">
+        <v>59.99</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="3"/>
+        <v>381.66666666666669</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="4"/>
+        <v>69.02</v>
+      </c>
+      <c r="I42" s="3">
+        <f t="shared" si="5"/>
+        <v>450.68666666666667</v>
+      </c>
+      <c r="K42" s="4">
+        <f t="shared" si="6"/>
+        <v>1352.06</v>
+      </c>
+      <c r="R42" s="4">
+        <f t="shared" si="10"/>
+        <v>1359.7399999999991</v>
+      </c>
       <c r="S42" s="5">
-        <f t="shared" si="10"/>
-        <v>-350.86999999999978</v>
+        <f t="shared" si="11"/>
+        <v>-0.18333333333310975</v>
+      </c>
+      <c r="W42" s="11">
+        <f t="shared" si="9"/>
+        <v>917.27666666666664</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.35">
@@ -2344,10 +2393,6 @@
       </c>
       <c r="C43" s="1">
         <v>1145</v>
-      </c>
-      <c r="S43" s="5">
-        <f t="shared" si="10"/>
-        <v>-350.86999999999978</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Calcualed Jan 2020 rent
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="34">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -371,12 +371,12 @@
   </sheetPr>
   <dimension ref="A1:X86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="K31" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C44" activeCellId="0" sqref="44:44"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="AC55" activeCellId="0" sqref="AC55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2386,7 +2386,7 @@
         <v>1145</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>45.6</v>
+        <v>63.6</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="false">D45</f>
@@ -2434,9 +2434,12 @@
       <c r="C47" s="1" t="n">
         <v>1145</v>
       </c>
+      <c r="D47" s="1" t="n">
+        <v>45.6</v>
+      </c>
       <c r="E47" s="1" t="n">
         <f aca="false">D46</f>
-        <v>45.6</v>
+        <v>63.6</v>
       </c>
       <c r="F47" s="1" t="n">
         <v>65.99</v>
@@ -2447,42 +2450,250 @@
       </c>
       <c r="H47" s="1" t="n">
         <f aca="false">(E47+F47)/3</f>
-        <v>37.1966666666667</v>
+        <v>43.1966666666667</v>
       </c>
       <c r="J47" s="2" t="n">
         <f aca="false">G47+H47</f>
-        <v>418.863333333333</v>
+        <v>424.863333333333</v>
       </c>
       <c r="L47" s="3" t="n">
         <f aca="false">3 *J47</f>
-        <v>1256.59</v>
+        <v>1274.59</v>
+      </c>
+      <c r="Q47" s="8" t="n">
+        <v>1389.8</v>
       </c>
       <c r="S47" s="3" t="n">
         <f aca="false">S46 + L47 - (J47 + M47+ N47 + O47 + P47 + Q47) + I47</f>
-        <v>2263.83666666667</v>
+        <v>886.036666666671</v>
       </c>
       <c r="T47" s="4" t="n">
         <f aca="false">T46 + J47 - M47</f>
-        <v>431.390000000002</v>
+        <v>437.390000000002</v>
       </c>
       <c r="X47" s="11" t="n">
         <f aca="false">X46 + J47 - Q47 + I47</f>
-        <v>1389.8</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.00000000000205</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C48" s="1" t="n">
         <v>1145</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="1" t="n">
+        <v>147.67</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <f aca="false">D47</f>
+        <v>45.6</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>65.99</v>
+      </c>
+      <c r="G48" s="9" t="n">
+        <f aca="false">C48/3</f>
+        <v>381.666666666667</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <f aca="false">(E48+F48)/3</f>
+        <v>37.1966666666667</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <f aca="false">G48+H48</f>
+        <v>418.863333333333</v>
+      </c>
+      <c r="L48" s="3" t="n">
+        <f aca="false">3 *J48</f>
+        <v>1256.59</v>
+      </c>
+      <c r="Q48" s="8" t="n">
+        <v>424.86</v>
+      </c>
+      <c r="S48" s="3" t="n">
+        <f aca="false">S47 + L48 - (J48 + M48+ N48 + O48 + P48 + Q48) + I48</f>
+        <v>1298.90333333334</v>
+      </c>
+      <c r="T48" s="4" t="n">
+        <f aca="false">T47 + J48 - M48</f>
+        <v>856.253333333335</v>
+      </c>
+      <c r="X48" s="11" t="n">
+        <f aca="false">X47 + J48 - Q48 + I48</f>
+        <v>0.00333333333537666</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C49" s="1" t="n">
+        <v>1145</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>149.67</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <f aca="false">D48</f>
+        <v>147.67</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>65.99</v>
+      </c>
+      <c r="G49" s="9" t="n">
+        <f aca="false">C49/3</f>
+        <v>381.666666666667</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <f aca="false">(E49+F49)/3</f>
+        <v>71.22</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <f aca="false">G49+H49</f>
+        <v>452.886666666667</v>
+      </c>
+      <c r="L49" s="3" t="n">
+        <f aca="false">3 *J49</f>
+        <v>1358.66</v>
+      </c>
+      <c r="S49" s="3" t="n">
+        <f aca="false">S48 + L49 - (J49 + M49+ N49 + O49 + P49 + Q49) + I49</f>
+        <v>2204.67666666667</v>
+      </c>
+      <c r="X49" s="11" t="n">
+        <f aca="false">X48 + J49 - Q49 + I49</f>
+        <v>452.890000000002</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>1145</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <f aca="false">D49</f>
+        <v>149.67</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>65.99</v>
+      </c>
+      <c r="G50" s="9" t="n">
+        <f aca="false">C50/3</f>
+        <v>381.666666666667</v>
+      </c>
+      <c r="H50" s="1" t="n">
+        <f aca="false">(E50+F50)/3</f>
+        <v>71.8866666666667</v>
+      </c>
+      <c r="J50" s="2" t="n">
+        <f aca="false">G50+H50</f>
+        <v>453.553333333333</v>
+      </c>
+      <c r="L50" s="3" t="n">
+        <f aca="false">3 *J50</f>
+        <v>1360.66</v>
+      </c>
+      <c r="S50" s="3" t="n">
+        <f aca="false">S49 + L50 - (J50 + M50+ N50 + O50 + P50 + Q50) + I50</f>
+        <v>3111.78333333334</v>
+      </c>
+      <c r="X50" s="11" t="n">
+        <f aca="false">X49 + J50 - Q50 + I50</f>
+        <v>906.443333333336</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="1" t="n">
         <v>1145</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding payments from jan 2020
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -372,11 +372,11 @@
   <dimension ref="A1:X86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K28" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="AC55" activeCellId="0" sqref="AC55"/>
+      <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="M49" activeCellId="0" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2558,9 +2558,16 @@
         <f aca="false">3 *J49</f>
         <v>1358.66</v>
       </c>
+      <c r="M49" s="4" t="n">
+        <v>3166</v>
+      </c>
       <c r="S49" s="3" t="n">
         <f aca="false">S48 + L49 - (J49 + M49+ N49 + O49 + P49 + Q49) + I49</f>
-        <v>2204.67666666667</v>
+        <v>-961.323333333327</v>
+      </c>
+      <c r="T49" s="4" t="n">
+        <f aca="false">T48 + J49 - M49</f>
+        <v>-1856.86</v>
       </c>
       <c r="X49" s="11" t="n">
         <f aca="false">X48 + J49 - Q49 + I49</f>
@@ -2600,13 +2607,20 @@
         <f aca="false">3 *J50</f>
         <v>1360.66</v>
       </c>
+      <c r="Q50" s="8" t="n">
+        <v>906.44</v>
+      </c>
       <c r="S50" s="3" t="n">
         <f aca="false">S49 + L50 - (J50 + M50+ N50 + O50 + P50 + Q50) + I50</f>
-        <v>3111.78333333334</v>
+        <v>-960.65666666666</v>
+      </c>
+      <c r="T50" s="4" t="n">
+        <f aca="false">T49 + J50 - M50</f>
+        <v>-1403.30666666666</v>
       </c>
       <c r="X50" s="11" t="n">
         <f aca="false">X49 + J50 - Q50 + I50</f>
-        <v>906.443333333336</v>
+        <v>0.00333333333492192</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added some June 2020 info
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrdie\Documents\Hayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B70A627-69D8-4BF7-ADE3-D21E975F050B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BAAF36-93BE-4487-8D38-1A755FF908EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="Q54" sqref="Q54"/>
+      <selection pane="bottomRight" activeCell="Q56" sqref="Q56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,26 +776,26 @@
         <v>87.26</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E52" si="0">D8</f>
+        <f t="shared" ref="E9:E54" si="0">D8</f>
         <v>79.540000000000006</v>
       </c>
       <c r="F9" s="1">
         <v>59.99</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ref="G9:G52" si="1">C9/3</f>
+        <f t="shared" ref="G9:G55" si="1">C9/3</f>
         <v>375</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H52" si="2">(E9+F9)/3</f>
+        <f t="shared" ref="H9:H55" si="2">(E9+F9)/3</f>
         <v>46.51</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ref="J9:J52" si="3">G9+H9</f>
+        <f t="shared" ref="J9:J55" si="3">G9+H9</f>
         <v>421.51</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" ref="L9:L52" si="4">3 *J9</f>
+        <f t="shared" ref="L9:L55" si="4">3 *J9</f>
         <v>1264.53</v>
       </c>
       <c r="M9" s="4">
@@ -2102,7 +2102,7 @@
         <v>1212.3166666666664</v>
       </c>
       <c r="T35" s="4">
-        <f t="shared" ref="T35:T52" si="10">T34 + J35 - M35</f>
+        <f t="shared" ref="T35:T55" si="10">T34 + J35 - M35</f>
         <v>769.6700000000003</v>
       </c>
       <c r="W35" s="7"/>
@@ -2457,7 +2457,7 @@
         <v>927.28</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" ref="S42:S52" si="12">S41 + L42 - (J42 + M42+ N42 + O42 + P42 + Q42) + I42</f>
+        <f t="shared" ref="S42:S55" si="12">S41 + L42 - (J42 + M42+ N42 + O42 + P42 + Q42) + I42</f>
         <v>437.45999999999935</v>
       </c>
       <c r="T42" s="4">
@@ -2465,7 +2465,7 @@
         <v>9.8166666666668903</v>
       </c>
       <c r="X42" s="11">
-        <f t="shared" ref="X42:X52" si="13">X41 + J42 - Q42 + I42</f>
+        <f t="shared" ref="X42:X55" si="13">X41 + J42 - Q42 + I42</f>
         <v>-15.003333333333217</v>
       </c>
     </row>
@@ -2930,6 +2930,9 @@
       <c r="C52" s="1">
         <v>1145</v>
       </c>
+      <c r="D52" s="1">
+        <v>164.8</v>
+      </c>
       <c r="E52" s="1">
         <f t="shared" si="0"/>
         <v>153.19</v>
@@ -2976,6 +2979,47 @@
       <c r="C53" s="1">
         <v>1145</v>
       </c>
+      <c r="D53" s="1">
+        <v>182.17</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="0"/>
+        <v>164.8</v>
+      </c>
+      <c r="F53" s="1">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="G53" s="9">
+        <f t="shared" si="1"/>
+        <v>381.66666666666669</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="2"/>
+        <v>76.930000000000007</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="3"/>
+        <v>458.59666666666669</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="4"/>
+        <v>1375.79</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>458.59</v>
+      </c>
+      <c r="S53" s="3">
+        <f t="shared" si="12"/>
+        <v>410.30333333333238</v>
+      </c>
+      <c r="T53" s="4">
+        <f t="shared" si="10"/>
+        <v>-32.346666666666351</v>
+      </c>
+      <c r="X53" s="11">
+        <f t="shared" si="13"/>
+        <v>3.3333333336145188E-3</v>
+      </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
@@ -2984,6 +3028,44 @@
       <c r="C54" s="1">
         <v>1145</v>
       </c>
+      <c r="E54" s="1">
+        <f t="shared" si="0"/>
+        <v>182.17</v>
+      </c>
+      <c r="F54" s="1">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="G54" s="9">
+        <f t="shared" si="1"/>
+        <v>381.66666666666669</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="2"/>
+        <v>82.719999999999985</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="3"/>
+        <v>464.38666666666666</v>
+      </c>
+      <c r="L54" s="3">
+        <f t="shared" si="4"/>
+        <v>1393.1599999999999</v>
+      </c>
+      <c r="Q54" s="8">
+        <v>464.39</v>
+      </c>
+      <c r="S54" s="3">
+        <f t="shared" si="12"/>
+        <v>874.68666666666559</v>
+      </c>
+      <c r="T54" s="4">
+        <f t="shared" si="10"/>
+        <v>432.0400000000003</v>
+      </c>
+      <c r="X54" s="11">
+        <f t="shared" si="13"/>
+        <v>2.8421709430404007E-13</v>
+      </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -2991,6 +3073,40 @@
       </c>
       <c r="C55" s="1">
         <v>1145</v>
+      </c>
+      <c r="F55" s="1">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="G55" s="9">
+        <f t="shared" si="1"/>
+        <v>381.66666666666669</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="2"/>
+        <v>21.996666666666666</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="3"/>
+        <v>403.66333333333336</v>
+      </c>
+      <c r="L55" s="3">
+        <f t="shared" si="4"/>
+        <v>1210.99</v>
+      </c>
+      <c r="Q55" s="8">
+        <v>403.66</v>
+      </c>
+      <c r="S55" s="3">
+        <f t="shared" si="12"/>
+        <v>1278.3533333333321</v>
+      </c>
+      <c r="T55" s="4">
+        <f t="shared" si="10"/>
+        <v>835.7033333333336</v>
+      </c>
+      <c r="X55" s="11">
+        <f t="shared" si="13"/>
+        <v>3.3333333336145188E-3</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started adding july 2020
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrdie\Documents\Hayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BAAF36-93BE-4487-8D38-1A755FF908EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E8DFB8-9786-42CF-BFE2-A30750248A80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="Q56" sqref="Q56"/>
+      <selection pane="bottomRight" activeCell="X56" sqref="X56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,19 +783,19 @@
         <v>59.99</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ref="G9:G55" si="1">C9/3</f>
+        <f t="shared" ref="G9:G56" si="1">C9/3</f>
         <v>375</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H55" si="2">(E9+F9)/3</f>
+        <f t="shared" ref="H9:H56" si="2">(E9+F9)/3</f>
         <v>46.51</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ref="J9:J55" si="3">G9+H9</f>
+        <f t="shared" ref="J9:J56" si="3">G9+H9</f>
         <v>421.51</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" ref="L9:L55" si="4">3 *J9</f>
+        <f t="shared" ref="L9:L56" si="4">3 *J9</f>
         <v>1264.53</v>
       </c>
       <c r="M9" s="4">
@@ -2102,7 +2102,7 @@
         <v>1212.3166666666664</v>
       </c>
       <c r="T35" s="4">
-        <f t="shared" ref="T35:T55" si="10">T34 + J35 - M35</f>
+        <f t="shared" ref="T35:T56" si="10">T34 + J35 - M35</f>
         <v>769.6700000000003</v>
       </c>
       <c r="W35" s="7"/>
@@ -2457,7 +2457,7 @@
         <v>927.28</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" ref="S42:S55" si="12">S41 + L42 - (J42 + M42+ N42 + O42 + P42 + Q42) + I42</f>
+        <f t="shared" ref="S42:S56" si="12">S41 + L42 - (J42 + M42+ N42 + O42 + P42 + Q42) + I42</f>
         <v>437.45999999999935</v>
       </c>
       <c r="T42" s="4">
@@ -2465,7 +2465,7 @@
         <v>9.8166666666668903</v>
       </c>
       <c r="X42" s="11">
-        <f t="shared" ref="X42:X55" si="13">X41 + J42 - Q42 + I42</f>
+        <f t="shared" ref="X42:X56" si="13">X41 + J42 - Q42 + I42</f>
         <v>-15.003333333333217</v>
       </c>
     </row>
@@ -3115,6 +3115,37 @@
       </c>
       <c r="C56" s="1">
         <v>1145</v>
+      </c>
+      <c r="F56" s="1">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="G56" s="9">
+        <f t="shared" si="1"/>
+        <v>381.66666666666669</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="2"/>
+        <v>21.996666666666666</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" si="3"/>
+        <v>403.66333333333336</v>
+      </c>
+      <c r="L56" s="3">
+        <f t="shared" si="4"/>
+        <v>1210.99</v>
+      </c>
+      <c r="S56" s="3">
+        <f t="shared" si="12"/>
+        <v>2085.6799999999989</v>
+      </c>
+      <c r="T56" s="4">
+        <f t="shared" si="10"/>
+        <v>1239.366666666667</v>
+      </c>
+      <c r="X56" s="11">
+        <f t="shared" si="13"/>
+        <v>403.66666666666697</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added payment from onno
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrdie\Documents\Hayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E8DFB8-9786-42CF-BFE2-A30750248A80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9AB458-82FA-4CB6-8D97-B8F7C24FD1D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -621,10 +623,10 @@
   <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="X56" sqref="X56"/>
+      <selection pane="bottomRight" activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,26 +778,26 @@
         <v>87.26</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ref="E9:E54" si="0">D8</f>
+        <f t="shared" ref="E9:E57" si="0">D8</f>
         <v>79.540000000000006</v>
       </c>
       <c r="F9" s="1">
         <v>59.99</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ref="G9:G56" si="1">C9/3</f>
+        <f t="shared" ref="G9:G57" si="1">C9/3</f>
         <v>375</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ref="H9:H56" si="2">(E9+F9)/3</f>
+        <f t="shared" ref="H9:H57" si="2">(E9+F9)/3</f>
         <v>46.51</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ref="J9:J56" si="3">G9+H9</f>
+        <f t="shared" ref="J9:J57" si="3">G9+H9</f>
         <v>421.51</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" ref="L9:L56" si="4">3 *J9</f>
+        <f t="shared" ref="L9:L57" si="4">3 *J9</f>
         <v>1264.53</v>
       </c>
       <c r="M9" s="4">
@@ -2102,7 +2104,7 @@
         <v>1212.3166666666664</v>
       </c>
       <c r="T35" s="4">
-        <f t="shared" ref="T35:T56" si="10">T34 + J35 - M35</f>
+        <f t="shared" ref="T35:T57" si="10">T34 + J35 - M35</f>
         <v>769.6700000000003</v>
       </c>
       <c r="W35" s="7"/>
@@ -2457,7 +2459,7 @@
         <v>927.28</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" ref="S42:S56" si="12">S41 + L42 - (J42 + M42+ N42 + O42 + P42 + Q42) + I42</f>
+        <f t="shared" ref="S42:S57" si="12">S41 + L42 - (J42 + M42+ N42 + O42 + P42 + Q42) + I42</f>
         <v>437.45999999999935</v>
       </c>
       <c r="T42" s="4">
@@ -2465,7 +2467,7 @@
         <v>9.8166666666668903</v>
       </c>
       <c r="X42" s="11">
-        <f t="shared" ref="X42:X56" si="13">X41 + J42 - Q42 + I42</f>
+        <f t="shared" ref="X42:X57" si="13">X41 + J42 - Q42 + I42</f>
         <v>-15.003333333333217</v>
       </c>
     </row>
@@ -3028,6 +3030,9 @@
       <c r="C54" s="1">
         <v>1145</v>
       </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
       <c r="E54" s="1">
         <f t="shared" si="0"/>
         <v>182.17</v>
@@ -3074,6 +3079,13 @@
       <c r="C55" s="1">
         <v>1145</v>
       </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F55" s="1">
         <v>65.989999999999995</v>
       </c>
@@ -3116,6 +3128,13 @@
       <c r="C56" s="1">
         <v>1145</v>
       </c>
+      <c r="D56" s="1">
+        <v>352.35</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F56" s="1">
         <v>65.989999999999995</v>
       </c>
@@ -3135,17 +3154,23 @@
         <f t="shared" si="4"/>
         <v>1210.99</v>
       </c>
+      <c r="M56" s="4">
+        <v>1760</v>
+      </c>
+      <c r="Q56" s="8">
+        <v>403.67</v>
+      </c>
       <c r="S56" s="3">
         <f t="shared" si="12"/>
-        <v>2085.6799999999989</v>
+        <v>-77.990000000001146</v>
       </c>
       <c r="T56" s="4">
         <f t="shared" si="10"/>
-        <v>1239.366666666667</v>
+        <v>-520.63333333333298</v>
       </c>
       <c r="X56" s="11">
         <f t="shared" si="13"/>
-        <v>403.66666666666697</v>
+        <v>-3.3333333330460846E-3</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -3154,6 +3179,41 @@
       </c>
       <c r="C57" s="1">
         <v>1145</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="0"/>
+        <v>352.35</v>
+      </c>
+      <c r="F57" s="1">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="G57" s="9">
+        <f t="shared" si="1"/>
+        <v>381.66666666666669</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="2"/>
+        <v>139.44666666666669</v>
+      </c>
+      <c r="J57" s="2">
+        <f t="shared" si="3"/>
+        <v>521.11333333333334</v>
+      </c>
+      <c r="L57" s="3">
+        <f t="shared" si="4"/>
+        <v>1563.3400000000001</v>
+      </c>
+      <c r="S57" s="3">
+        <f t="shared" si="12"/>
+        <v>964.23666666666566</v>
+      </c>
+      <c r="T57" s="4">
+        <f t="shared" si="10"/>
+        <v>0.48000000000035925</v>
+      </c>
+      <c r="X57" s="11">
+        <f t="shared" si="13"/>
+        <v>521.11000000000035</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added power for november
</commit_message>
<xml_diff>
--- a/rent.xlsx
+++ b/rent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byrdie\Documents\Hayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B151EF8-B048-42E1-A827-5A177B791C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189EDE4F-B39A-47C4-BB0B-2EB717D5FF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -222,14 +222,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -620,10 +620,10 @@
   <dimension ref="A1:BM61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="A59" sqref="A59:XFD59"/>
+      <selection pane="bottomRight" activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,14 +837,14 @@
         <v>59.99</v>
       </c>
       <c r="F9" s="1">
-        <f>C9 + D9 + E9</f>
+        <f t="shared" ref="F9:F40" si="0">C9 + D9 + E9</f>
         <v>1265.02</v>
       </c>
       <c r="I9" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J9" s="5">
-        <f>I9*F9</f>
+        <f t="shared" ref="J9:J40" si="1">I9*F9</f>
         <v>421.67333333333329</v>
       </c>
       <c r="K9" s="2">
@@ -861,7 +861,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="U9" s="5">
-        <f>T9*F9</f>
+        <f t="shared" ref="U9:U40" si="2">T9*F9</f>
         <v>421.67333333333329</v>
       </c>
       <c r="V9" s="3">
@@ -876,7 +876,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="Z9" s="5">
-        <f>Y9*F9</f>
+        <f t="shared" ref="Z9:Z18" si="3">Y9*F9</f>
         <v>421.67333333333329</v>
       </c>
       <c r="AA9" s="3">
@@ -901,53 +901,53 @@
         <v>59.99</v>
       </c>
       <c r="F10" s="1">
-        <f>C10 + D10 + E10</f>
+        <f t="shared" si="0"/>
         <v>1273.32</v>
       </c>
       <c r="I10" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J10" s="5">
-        <f>I10*F10</f>
+        <f t="shared" si="1"/>
         <v>424.43999999999994</v>
       </c>
       <c r="K10" s="2">
-        <f t="shared" ref="K10:K60" si="0">-F10-O10</f>
+        <f t="shared" ref="K10:K61" si="4">-F10-O10</f>
         <v>-1273.32</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" ref="L10:L60" si="1">L9+K10+J10+Q10+V10+AA10+AF10+AK10</f>
+        <f t="shared" ref="L10:L61" si="5">L9+K10+J10+Q10+V10+AA10+AF10+AK10</f>
         <v>-2.2266666666665742</v>
       </c>
       <c r="M10" s="5"/>
       <c r="T10" s="7">
-        <f t="shared" ref="T10:Y59" si="2">1/3</f>
+        <f t="shared" ref="T10:Y59" si="6">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="U10" s="5">
-        <f>T10*F10</f>
+        <f t="shared" si="2"/>
         <v>424.43999999999994</v>
       </c>
       <c r="V10" s="3">
         <v>424</v>
       </c>
       <c r="W10" s="5">
-        <f t="shared" ref="W10:W60" si="3">W9-U10+V10</f>
+        <f t="shared" ref="W10:W59" si="7">W9-U10+V10</f>
         <v>-2.1133333333332303</v>
       </c>
       <c r="Y10" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="Z10" s="5">
-        <f>Y10*F10</f>
+        <f t="shared" si="3"/>
         <v>424.43999999999994</v>
       </c>
       <c r="AA10" s="3">
         <v>424</v>
       </c>
       <c r="AB10" s="5">
-        <f t="shared" ref="AB10:AB60" si="4">AB9-Z10+AA10</f>
+        <f t="shared" ref="AB10:AB18" si="8">AB9-Z10+AA10</f>
         <v>-0.11333333333323026</v>
       </c>
     </row>
@@ -965,50 +965,50 @@
         <v>59.99</v>
       </c>
       <c r="F11" s="1">
-        <f>C11 + D11 + E11</f>
+        <f t="shared" si="0"/>
         <v>1286.94</v>
       </c>
       <c r="I11" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J11" s="5">
-        <f>I11*F11</f>
+        <f t="shared" si="1"/>
         <v>428.98</v>
       </c>
       <c r="K11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1286.94</v>
       </c>
       <c r="L11" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-438.51666666666648</v>
       </c>
       <c r="M11" s="5"/>
       <c r="T11" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U11" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U11" s="5">
-        <f>T11*F11</f>
         <v>428.98</v>
       </c>
       <c r="W11" s="5">
+        <f t="shared" si="7"/>
+        <v>-431.09333333333325</v>
+      </c>
+      <c r="Y11" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z11" s="5">
         <f t="shared" si="3"/>
-        <v>-431.09333333333325</v>
-      </c>
-      <c r="Y11" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z11" s="5">
-        <f>Y11*F11</f>
         <v>428.98</v>
       </c>
       <c r="AA11" s="3">
         <v>421.67</v>
       </c>
       <c r="AB11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-7.4233333333332325</v>
       </c>
     </row>
@@ -1026,47 +1026,47 @@
         <v>59.99</v>
       </c>
       <c r="F12" s="1">
-        <f>C12 + D12 + E12</f>
+        <f t="shared" si="0"/>
         <v>1320.8</v>
       </c>
       <c r="I12" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J12" s="5">
-        <f>I12*F12</f>
+        <f t="shared" si="1"/>
         <v>440.26666666666665</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1320.8</v>
       </c>
       <c r="L12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1319.0499999999997</v>
       </c>
       <c r="M12" s="5"/>
       <c r="T12" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U12" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U12" s="5">
-        <f>T12*F12</f>
         <v>440.26666666666665</v>
       </c>
       <c r="W12" s="5">
+        <f t="shared" si="7"/>
+        <v>-871.3599999999999</v>
+      </c>
+      <c r="Y12" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z12" s="5">
         <f t="shared" si="3"/>
-        <v>-871.3599999999999</v>
-      </c>
-      <c r="Y12" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z12" s="5">
-        <f>Y12*F12</f>
         <v>440.26666666666665</v>
       </c>
       <c r="AB12" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-447.68999999999988</v>
       </c>
     </row>
@@ -1084,53 +1084,53 @@
         <v>59.99</v>
       </c>
       <c r="F13" s="1">
-        <f>C13 + D13 + E13</f>
+        <f t="shared" si="0"/>
         <v>1376.53</v>
       </c>
       <c r="I13" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J13" s="5">
-        <f>I13*F13</f>
+        <f t="shared" si="1"/>
         <v>458.84333333333331</v>
       </c>
       <c r="K13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1376.53</v>
       </c>
       <c r="L13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-532.73666666666668</v>
       </c>
       <c r="M13" s="5"/>
       <c r="T13" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U13" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U13" s="5">
-        <f>T13*F13</f>
         <v>458.84333333333331</v>
       </c>
       <c r="V13" s="3">
         <v>850</v>
       </c>
       <c r="W13" s="5">
+        <f t="shared" si="7"/>
+        <v>-480.20333333333315</v>
+      </c>
+      <c r="Y13" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z13" s="5">
         <f t="shared" si="3"/>
-        <v>-480.20333333333315</v>
-      </c>
-      <c r="Y13" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z13" s="5">
-        <f>Y13*F13</f>
         <v>458.84333333333331</v>
       </c>
       <c r="AA13" s="3">
         <v>854</v>
       </c>
       <c r="AB13" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-52.533333333333189</v>
       </c>
     </row>
@@ -1151,47 +1151,47 @@
         <v>59.99</v>
       </c>
       <c r="F14" s="1">
-        <f>C14 + D14 + E14</f>
+        <f t="shared" si="0"/>
         <v>1399.47</v>
       </c>
       <c r="I14" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J14" s="5">
-        <f>I14*F14</f>
+        <f t="shared" si="1"/>
         <v>466.49</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1399.47</v>
       </c>
       <c r="L14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1465.7166666666667</v>
       </c>
       <c r="M14" s="5"/>
       <c r="T14" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U14" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U14" s="5">
-        <f>T14*F14</f>
         <v>466.49</v>
       </c>
       <c r="W14" s="5">
+        <f t="shared" si="7"/>
+        <v>-946.69333333333316</v>
+      </c>
+      <c r="Y14" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z14" s="5">
         <f t="shared" si="3"/>
-        <v>-946.69333333333316</v>
-      </c>
-      <c r="Y14" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z14" s="5">
-        <f>Y14*F14</f>
         <v>466.49</v>
       </c>
       <c r="AB14" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-519.0233333333332</v>
       </c>
     </row>
@@ -1209,53 +1209,53 @@
         <v>59.99</v>
       </c>
       <c r="F15" s="1">
-        <f>C15 + D15 + E15</f>
+        <f t="shared" si="0"/>
         <v>1184.99</v>
       </c>
       <c r="I15" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J15" s="5">
-        <f>I15*F15</f>
+        <f t="shared" si="1"/>
         <v>394.99666666666667</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1184.99</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-28.600000000000023</v>
       </c>
       <c r="M15" s="5"/>
       <c r="T15" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U15" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U15" s="5">
-        <f>T15*F15</f>
         <v>394.99666666666667</v>
       </c>
       <c r="V15" s="3">
         <v>1328</v>
       </c>
       <c r="W15" s="5">
+        <f t="shared" si="7"/>
+        <v>-13.689999999999827</v>
+      </c>
+      <c r="Y15" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z15" s="5">
         <f t="shared" si="3"/>
-        <v>-13.689999999999827</v>
-      </c>
-      <c r="Y15" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z15" s="5">
-        <f>Y15*F15</f>
         <v>394.99666666666667</v>
       </c>
       <c r="AA15" s="3">
         <v>899.11</v>
       </c>
       <c r="AB15" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-14.909999999999854</v>
       </c>
     </row>
@@ -1273,53 +1273,53 @@
         <v>59.99</v>
       </c>
       <c r="F16" s="1">
-        <f>C16 + D16 + E16</f>
+        <f t="shared" si="0"/>
         <v>1456.08</v>
       </c>
       <c r="I16" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J16" s="5">
-        <f>I16*F16</f>
+        <f t="shared" si="1"/>
         <v>485.35999999999996</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1456.08</v>
       </c>
       <c r="L16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-66.319999999999936</v>
       </c>
       <c r="M16" s="5"/>
       <c r="T16" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U16" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U16" s="5">
-        <f>T16*F16</f>
         <v>485.35999999999996</v>
       </c>
       <c r="V16" s="3">
         <v>466.5</v>
       </c>
       <c r="W16" s="5">
+        <f t="shared" si="7"/>
+        <v>-32.549999999999784</v>
+      </c>
+      <c r="Y16" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z16" s="5">
         <f t="shared" si="3"/>
-        <v>-32.549999999999784</v>
-      </c>
-      <c r="Y16" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z16" s="5">
-        <f>Y16*F16</f>
         <v>485.35999999999996</v>
       </c>
       <c r="AA16" s="3">
         <v>466.5</v>
       </c>
       <c r="AB16" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-33.769999999999811</v>
       </c>
     </row>
@@ -1337,47 +1337,47 @@
         <v>59.99</v>
       </c>
       <c r="F17" s="1">
-        <f>C17 + D17 + E17</f>
+        <f t="shared" si="0"/>
         <v>1301.1099999999999</v>
       </c>
       <c r="I17" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J17" s="5">
-        <f>I17*F17</f>
+        <f t="shared" si="1"/>
         <v>433.70333333333326</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1301.1099999999999</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-933.72666666666657</v>
       </c>
       <c r="M17" s="5"/>
       <c r="T17" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U17" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U17" s="5">
-        <f>T17*F17</f>
         <v>433.70333333333326</v>
       </c>
       <c r="W17" s="5">
+        <f t="shared" si="7"/>
+        <v>-466.25333333333305</v>
+      </c>
+      <c r="Y17" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z17" s="5">
         <f t="shared" si="3"/>
-        <v>-466.25333333333305</v>
-      </c>
-      <c r="Y17" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z17" s="5">
-        <f>Y17*F17</f>
         <v>433.70333333333326</v>
       </c>
       <c r="AB17" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-467.47333333333307</v>
       </c>
     </row>
@@ -1395,50 +1395,50 @@
         <v>59.99</v>
       </c>
       <c r="F18" s="1">
-        <f>C18 + D18 + E18</f>
+        <f t="shared" si="0"/>
         <v>1291.95</v>
       </c>
       <c r="I18" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J18" s="5">
-        <f>I18*F18</f>
+        <f t="shared" si="1"/>
         <v>430.65</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1291.95</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-914.66666666666663</v>
       </c>
       <c r="M18" s="5"/>
       <c r="T18" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U18" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U18" s="5">
-        <f>T18*F18</f>
         <v>430.65</v>
       </c>
       <c r="W18" s="5">
+        <f t="shared" si="7"/>
+        <v>-896.90333333333297</v>
+      </c>
+      <c r="Y18" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Z18" s="5">
         <f t="shared" si="3"/>
-        <v>-896.90333333333297</v>
-      </c>
-      <c r="Y18" s="7">
-        <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="Z18" s="5">
-        <f>Y18*F18</f>
         <v>430.65</v>
       </c>
       <c r="AA18" s="3">
         <v>880.36</v>
       </c>
       <c r="AB18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-17.76333333333298</v>
       </c>
     </row>
@@ -1456,35 +1456,35 @@
         <v>59.99</v>
       </c>
       <c r="F19" s="1">
-        <f>C19 + D19 + E19</f>
+        <f t="shared" si="0"/>
         <v>1256.99</v>
       </c>
       <c r="I19" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J19" s="5">
-        <f>I19*F19</f>
+        <f t="shared" si="1"/>
         <v>418.99666666666667</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1256.99</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1752.66</v>
       </c>
       <c r="M19" s="5"/>
       <c r="T19" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U19" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U19" s="5">
-        <f>T19*F19</f>
         <v>418.99666666666667</v>
       </c>
       <c r="W19" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1315.8999999999996</v>
       </c>
       <c r="AD19" s="7">
@@ -1492,7 +1492,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="AE19" s="5">
-        <f>AD19*F19</f>
+        <f t="shared" ref="AE19:AE34" si="9">AD19*F19</f>
         <v>418.99666666666667</v>
       </c>
       <c r="AG19" s="5">
@@ -1514,53 +1514,53 @@
         <v>59.99</v>
       </c>
       <c r="F20" s="1">
-        <f>C20 + D20 + E20</f>
+        <f t="shared" si="0"/>
         <v>1257.3599999999999</v>
       </c>
       <c r="I20" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J20" s="5">
-        <f>I20*F20</f>
+        <f t="shared" si="1"/>
         <v>419.11999999999995</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1257.3599999999999</v>
       </c>
       <c r="L20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-402.48000000000013</v>
       </c>
       <c r="M20" s="5"/>
       <c r="T20" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U20" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U20" s="5">
-        <f>T20*F20</f>
         <v>419.11999999999995</v>
       </c>
       <c r="V20" s="3">
         <v>1324.06</v>
       </c>
       <c r="W20" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-410.95999999999958</v>
       </c>
       <c r="AD20" s="7">
-        <f t="shared" ref="AD20:AI34" si="5">1/3</f>
+        <f t="shared" ref="AD20:AI34" si="10">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE20" s="5">
-        <f>AD20*F20</f>
+        <f t="shared" si="9"/>
         <v>419.11999999999995</v>
       </c>
       <c r="AF20" s="3">
         <v>864.36</v>
       </c>
       <c r="AG20" s="5">
-        <f t="shared" ref="AG20:AG60" si="6">AG19-AE20+AF20</f>
+        <f t="shared" ref="AG20:AG34" si="11">AG19-AE20+AF20</f>
         <v>26.243333333333453</v>
       </c>
     </row>
@@ -1578,47 +1578,47 @@
         <v>59.99</v>
       </c>
       <c r="F21" s="1">
-        <f>C21 + D21 + E21</f>
+        <f t="shared" si="0"/>
         <v>1256.69</v>
       </c>
       <c r="I21" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J21" s="5">
-        <f>I21*F21</f>
+        <f t="shared" si="1"/>
         <v>418.89666666666665</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1256.69</v>
       </c>
       <c r="L21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1240.2733333333335</v>
       </c>
       <c r="M21" s="5"/>
       <c r="T21" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U21" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U21" s="5">
-        <f>T21*F21</f>
         <v>418.89666666666665</v>
       </c>
       <c r="W21" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-829.85666666666623</v>
       </c>
       <c r="AD21" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE21" s="5">
-        <f>AD21*F21</f>
+        <f t="shared" si="9"/>
         <v>418.89666666666665</v>
       </c>
       <c r="AG21" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-392.65333333333319</v>
       </c>
     </row>
@@ -1636,53 +1636,53 @@
         <v>59.99</v>
       </c>
       <c r="F22" s="1">
-        <f>C22 + D22 + E22</f>
+        <f t="shared" si="0"/>
         <v>1284.24</v>
       </c>
       <c r="I22" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J22" s="5">
-        <f>I22*F22</f>
+        <f t="shared" si="1"/>
         <v>428.08</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1284.24</v>
       </c>
       <c r="L22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>348.35666666666657</v>
       </c>
       <c r="M22" s="5"/>
       <c r="T22" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U22" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U22" s="5">
-        <f>T22*F22</f>
         <v>428.08</v>
       </c>
       <c r="V22" s="3">
         <v>1600</v>
       </c>
       <c r="W22" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>342.06333333333373</v>
       </c>
       <c r="AD22" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE22" s="5">
-        <f>AD22*F22</f>
+        <f t="shared" si="9"/>
         <v>428.08</v>
       </c>
       <c r="AF22" s="3">
         <v>844.79</v>
       </c>
       <c r="AG22" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>24.056666666666843</v>
       </c>
     </row>
@@ -1700,47 +1700,47 @@
         <v>59.99</v>
       </c>
       <c r="F23" s="1">
-        <f>C23 + D23 + E23</f>
+        <f t="shared" si="0"/>
         <v>1340.02</v>
       </c>
       <c r="I23" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J23" s="5">
-        <f>I23*F23</f>
+        <f t="shared" si="1"/>
         <v>446.67333333333329</v>
       </c>
       <c r="K23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1340.02</v>
       </c>
       <c r="L23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-544.99000000000012</v>
       </c>
       <c r="M23" s="5"/>
       <c r="T23" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U23" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U23" s="5">
-        <f>T23*F23</f>
         <v>446.67333333333329</v>
       </c>
       <c r="W23" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-104.60999999999956</v>
       </c>
       <c r="AD23" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE23" s="5">
-        <f>AD23*F23</f>
+        <f t="shared" si="9"/>
         <v>446.67333333333329</v>
       </c>
       <c r="AG23" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-422.61666666666645</v>
       </c>
     </row>
@@ -1758,50 +1758,50 @@
         <v>59.99</v>
       </c>
       <c r="F24" s="1">
-        <f>C24 + D24 + E24</f>
+        <f t="shared" si="0"/>
         <v>1363.98</v>
       </c>
       <c r="I24" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J24" s="5">
-        <f>I24*F24</f>
+        <f t="shared" si="1"/>
         <v>454.65999999999997</v>
       </c>
       <c r="K24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1363.98</v>
       </c>
       <c r="L24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-543.3100000000004</v>
       </c>
       <c r="M24" s="5"/>
       <c r="T24" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U24" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U24" s="5">
-        <f>T24*F24</f>
         <v>454.65999999999997</v>
       </c>
       <c r="W24" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-559.26999999999953</v>
       </c>
       <c r="AD24" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE24" s="5">
-        <f>AD24*F24</f>
+        <f t="shared" si="9"/>
         <v>454.65999999999997</v>
       </c>
       <c r="AF24" s="3">
         <v>911</v>
       </c>
       <c r="AG24" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>33.723333333333585</v>
       </c>
     </row>
@@ -1819,47 +1819,47 @@
         <v>59.99</v>
       </c>
       <c r="F25" s="1">
-        <f>C25 + D25 + E25</f>
+        <f t="shared" si="0"/>
         <v>1355.1299999999999</v>
       </c>
       <c r="I25" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J25" s="5">
-        <f>I25*F25</f>
+        <f t="shared" si="1"/>
         <v>451.70999999999992</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1355.1299999999999</v>
       </c>
       <c r="L25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1446.7300000000005</v>
       </c>
       <c r="M25" s="5"/>
       <c r="T25" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U25" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U25" s="5">
-        <f>T25*F25</f>
         <v>451.70999999999992</v>
       </c>
       <c r="W25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1010.9799999999994</v>
       </c>
       <c r="AD25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE25" s="5">
-        <f>AD25*F25</f>
+        <f t="shared" si="9"/>
         <v>451.70999999999992</v>
       </c>
       <c r="AG25" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-417.98666666666634</v>
       </c>
     </row>
@@ -1880,50 +1880,50 @@
         <v>59.99</v>
       </c>
       <c r="F26" s="1">
-        <f>C26 + D26 + E26</f>
+        <f t="shared" si="0"/>
         <v>1362.98</v>
       </c>
       <c r="I26" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J26" s="5">
-        <f>I26*F26</f>
+        <f t="shared" si="1"/>
         <v>454.32666666666665</v>
       </c>
       <c r="K26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1362.98</v>
       </c>
       <c r="L26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1255.3833333333337</v>
       </c>
       <c r="M26" s="5"/>
       <c r="T26" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U26" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U26" s="5">
-        <f>T26*F26</f>
         <v>454.32666666666665</v>
       </c>
       <c r="V26" s="3">
         <v>1100</v>
       </c>
       <c r="W26" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-365.30666666666616</v>
       </c>
       <c r="AD26" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE26" s="5">
-        <f>AD26*F26</f>
+        <f t="shared" si="9"/>
         <v>454.32666666666665</v>
       </c>
       <c r="AG26" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-872.31333333333305</v>
       </c>
     </row>
@@ -1941,50 +1941,50 @@
         <v>59.99</v>
       </c>
       <c r="F27" s="1">
-        <f>C27 + D27 + E27</f>
+        <f t="shared" si="0"/>
         <v>1382.53</v>
       </c>
       <c r="I27" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J27" s="5">
-        <f>I27*F27</f>
+        <f t="shared" si="1"/>
         <v>460.84333333333331</v>
       </c>
       <c r="K27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1382.53</v>
       </c>
       <c r="L27" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1677.0700000000006</v>
       </c>
       <c r="M27" s="5"/>
       <c r="T27" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U27" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U27" s="5">
-        <f>T27*F27</f>
         <v>460.84333333333331</v>
       </c>
       <c r="W27" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-826.14999999999941</v>
       </c>
       <c r="AD27" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE27" s="5">
-        <f>AD27*F27</f>
+        <f t="shared" si="9"/>
         <v>460.84333333333331</v>
       </c>
       <c r="AF27" s="3">
         <v>500</v>
       </c>
       <c r="AG27" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-833.1566666666663</v>
       </c>
     </row>
@@ -2002,53 +2002,53 @@
         <v>59.99</v>
       </c>
       <c r="F28" s="1">
-        <f>C28 + D28 + E28</f>
+        <f t="shared" si="0"/>
         <v>1369.29</v>
       </c>
       <c r="I28" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J28" s="5">
-        <f>I28*F28</f>
+        <f t="shared" si="1"/>
         <v>456.42999999999995</v>
       </c>
       <c r="K28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1369.29</v>
       </c>
       <c r="L28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>380.06999999999925</v>
       </c>
       <c r="M28" s="5"/>
       <c r="T28" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U28" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U28" s="5">
-        <f>T28*F28</f>
         <v>456.42999999999995</v>
       </c>
       <c r="V28" s="3">
         <v>1800</v>
       </c>
       <c r="W28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>517.42000000000053</v>
       </c>
       <c r="AD28" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE28" s="5">
-        <f>AD28*F28</f>
+        <f t="shared" si="9"/>
         <v>456.42999999999995</v>
       </c>
       <c r="AF28" s="3">
         <v>1170</v>
       </c>
       <c r="AG28" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-119.58666666666613</v>
       </c>
     </row>
@@ -2066,47 +2066,47 @@
         <v>59.99</v>
       </c>
       <c r="F29" s="1">
-        <f>C29 + D29 + E29</f>
+        <f t="shared" si="0"/>
         <v>1334.43</v>
       </c>
       <c r="I29" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J29" s="5">
-        <f>I29*F29</f>
+        <f t="shared" si="1"/>
         <v>444.81</v>
       </c>
       <c r="K29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1334.43</v>
       </c>
       <c r="L29" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-509.55000000000081</v>
       </c>
       <c r="M29" s="5"/>
       <c r="T29" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U29" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U29" s="5">
-        <f>T29*F29</f>
         <v>444.81</v>
       </c>
       <c r="W29" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>72.610000000000525</v>
       </c>
       <c r="AD29" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE29" s="5">
-        <f>AD29*F29</f>
+        <f t="shared" si="9"/>
         <v>444.81</v>
       </c>
       <c r="AG29" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-564.39666666666608</v>
       </c>
     </row>
@@ -2124,50 +2124,50 @@
         <v>59.99</v>
       </c>
       <c r="F30" s="1">
-        <f>C30 + D30 + E30</f>
+        <f t="shared" si="0"/>
         <v>1307.1600000000001</v>
       </c>
       <c r="I30" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J30" s="5">
-        <f>I30*F30</f>
+        <f t="shared" si="1"/>
         <v>435.72</v>
       </c>
       <c r="K30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1307.1600000000001</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-380.99000000000092</v>
       </c>
       <c r="M30" s="5"/>
       <c r="T30" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U30" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U30" s="5">
-        <f>T30*F30</f>
         <v>435.72</v>
       </c>
       <c r="W30" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-363.1099999999995</v>
       </c>
       <c r="AD30" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE30" s="5">
-        <f>AD30*F30</f>
+        <f t="shared" si="9"/>
         <v>435.72</v>
       </c>
       <c r="AF30" s="3">
         <v>1000</v>
       </c>
       <c r="AG30" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>-0.11666666666610581</v>
       </c>
       <c r="BJ30" s="3"/>
@@ -2186,22 +2186,22 @@
         <v>59.99</v>
       </c>
       <c r="F31" s="1">
-        <f>C31 + D31 + E31</f>
+        <f t="shared" si="0"/>
         <v>1280.0899999999999</v>
       </c>
       <c r="I31" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J31" s="5">
-        <f>I31*F31</f>
+        <f t="shared" si="1"/>
         <v>426.6966666666666</v>
       </c>
       <c r="K31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1280.0899999999999</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-344.76333333333417</v>
       </c>
       <c r="M31" s="5"/>
@@ -2209,30 +2209,30 @@
         <v>0</v>
       </c>
       <c r="U31" s="5">
-        <f>T31*F31</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W31" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-363.1099999999995</v>
       </c>
       <c r="AD31" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE31" s="5">
-        <f>AD31*F31</f>
+        <f t="shared" si="9"/>
         <v>426.6966666666666</v>
       </c>
       <c r="AF31" s="3">
         <v>444.81</v>
       </c>
       <c r="AG31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>17.996666666667295</v>
       </c>
       <c r="AI31" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AJ31" s="5">
@@ -2262,22 +2262,22 @@
         <v>59.99</v>
       </c>
       <c r="F32" s="1">
-        <f>C32 + D32 + E32</f>
+        <f t="shared" si="0"/>
         <v>1299.56</v>
       </c>
       <c r="I32" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J32" s="5">
-        <f>I32*F32</f>
+        <f t="shared" si="1"/>
         <v>433.18666666666661</v>
       </c>
       <c r="K32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1299.56</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-338.13666666666768</v>
       </c>
       <c r="M32" s="5"/>
@@ -2285,30 +2285,30 @@
         <v>0</v>
       </c>
       <c r="U32" s="5">
-        <f>T32*F32</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-363.1099999999995</v>
       </c>
       <c r="AD32" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE32" s="5">
-        <f>AD32*F32</f>
+        <f t="shared" si="9"/>
         <v>433.18666666666661</v>
       </c>
       <c r="AF32" s="3">
         <v>433</v>
       </c>
       <c r="AG32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>17.810000000000684</v>
       </c>
       <c r="AI32" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AJ32" s="5">
@@ -2319,7 +2319,7 @@
         <v>440</v>
       </c>
       <c r="AL32" s="5">
-        <f t="shared" ref="AL32:AL60" si="7">AL31-AJ32+AK32</f>
+        <f t="shared" ref="AL32:AL34" si="12">AL31-AJ32+AK32</f>
         <v>24.92666666666679</v>
       </c>
       <c r="BJ32" s="3"/>
@@ -2338,22 +2338,22 @@
         <v>59.99</v>
       </c>
       <c r="F33" s="1">
-        <f>C33 + D33 + E33</f>
+        <f t="shared" si="0"/>
         <v>1284.49</v>
       </c>
       <c r="I33" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J33" s="5">
-        <f>I33*F33</f>
+        <f t="shared" si="1"/>
         <v>428.1633333333333</v>
       </c>
       <c r="K33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1284.49</v>
       </c>
       <c r="L33" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-334.4633333333345</v>
       </c>
       <c r="M33" s="5"/>
@@ -2361,30 +2361,30 @@
         <v>0</v>
       </c>
       <c r="U33" s="5">
-        <f>T33*F33</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-363.1099999999995</v>
       </c>
       <c r="AD33" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE33" s="5">
-        <f>AD33*F33</f>
+        <f t="shared" si="9"/>
         <v>428.1633333333333</v>
       </c>
       <c r="AF33" s="3">
         <v>440</v>
       </c>
       <c r="AG33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>29.646666666667386</v>
       </c>
       <c r="AI33" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AJ33" s="5">
@@ -2395,7 +2395,7 @@
         <v>420</v>
       </c>
       <c r="AL33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>16.763333333333492</v>
       </c>
       <c r="BJ33" s="3"/>
@@ -2414,22 +2414,22 @@
         <v>59.99</v>
       </c>
       <c r="F34" s="1">
-        <f>C34 + D34 + E34</f>
+        <f t="shared" si="0"/>
         <v>1293.8599999999999</v>
       </c>
       <c r="I34" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J34" s="5">
-        <f>I34*F34</f>
+        <f t="shared" si="1"/>
         <v>431.28666666666663</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1293.8599999999999</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-357.03666666666777</v>
       </c>
       <c r="M34" s="5"/>
@@ -2437,30 +2437,30 @@
         <v>0</v>
       </c>
       <c r="U34" s="5">
-        <f>T34*F34</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-363.1099999999995</v>
       </c>
       <c r="AD34" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AE34" s="5">
-        <f>AD34*F34</f>
+        <f t="shared" si="9"/>
         <v>431.28666666666663</v>
       </c>
       <c r="AF34" s="3">
         <v>420</v>
       </c>
       <c r="AG34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>18.360000000000753</v>
       </c>
       <c r="AI34" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="AJ34" s="5">
@@ -2471,7 +2471,7 @@
         <v>420</v>
       </c>
       <c r="AL34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5.4766666666668584</v>
       </c>
       <c r="BJ34" s="3"/>
@@ -2490,7 +2490,7 @@
         <v>59.99</v>
       </c>
       <c r="F35" s="1">
-        <f>C35 + D35 + E35</f>
+        <f t="shared" si="0"/>
         <v>1309.94</v>
       </c>
       <c r="I35" s="8">
@@ -2498,15 +2498,15 @@
         <v>0.5</v>
       </c>
       <c r="J35" s="5">
-        <f>I35*F35</f>
+        <f t="shared" si="1"/>
         <v>654.97</v>
       </c>
       <c r="K35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1309.94</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1012.0066666666678</v>
       </c>
       <c r="M35" s="5"/>
@@ -2515,11 +2515,11 @@
         <v>0.5</v>
       </c>
       <c r="U35" s="5">
-        <f>T35*F35</f>
+        <f t="shared" si="2"/>
         <v>654.97</v>
       </c>
       <c r="W35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1018.0799999999995</v>
       </c>
       <c r="AG35" s="5"/>
@@ -2539,31 +2539,31 @@
         <v>59.99</v>
       </c>
       <c r="F36" s="1">
-        <f>C36 + D36 + E36</f>
+        <f t="shared" si="0"/>
         <v>1335.51</v>
       </c>
       <c r="I36" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J36" s="5">
-        <f>I36*F36</f>
+        <f t="shared" si="1"/>
         <v>445.16999999999996</v>
       </c>
       <c r="K36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1335.51</v>
       </c>
       <c r="L36" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2279.3233333333324</v>
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="7">
-        <f t="shared" ref="N36:N59" si="8">1/3</f>
+        <f t="shared" ref="N36:N59" si="13">1/3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="P36" s="5">
-        <f>N36*F36 + O36</f>
+        <f t="shared" ref="P36:P61" si="14">N36*F36 + O36</f>
         <v>445.16999999999996</v>
       </c>
       <c r="Q36" s="10">
@@ -2575,18 +2575,18 @@
         <v>-63.499999999999943</v>
       </c>
       <c r="T36" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U36" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U36" s="5">
-        <f>T36*F36</f>
         <v>445.16999999999996</v>
       </c>
       <c r="V36" s="3">
         <v>3800</v>
       </c>
       <c r="W36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2336.7500000000005</v>
       </c>
       <c r="AG36" s="5"/>
@@ -2607,31 +2607,31 @@
         <v>59.99</v>
       </c>
       <c r="F37" s="1">
-        <f>C37 + D37 + E37</f>
+        <f t="shared" si="0"/>
         <v>1332.99</v>
       </c>
       <c r="I37" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J37" s="5">
-        <f>I37*F37</f>
+        <f t="shared" si="1"/>
         <v>444.33</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1332.99</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1876.9233333333323</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P37" s="5">
-        <f>N37*F37 + O37</f>
+        <f t="shared" si="14"/>
         <v>444.33</v>
       </c>
       <c r="Q37" s="10">
@@ -2639,19 +2639,19 @@
         <v>486.26</v>
       </c>
       <c r="R37" s="5">
-        <f t="shared" ref="R37:R60" si="9">R36-P37+Q37</f>
+        <f t="shared" ref="R37:R61" si="15">R36-P37+Q37</f>
         <v>-21.569999999999936</v>
       </c>
       <c r="T37" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U37" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U37" s="5">
-        <f>T37*F37</f>
         <v>444.33</v>
       </c>
       <c r="W37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1892.4200000000005</v>
       </c>
       <c r="AG37" s="5"/>
@@ -2674,31 +2674,31 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F38" s="1">
-        <f>C38 + D38 + E38</f>
+        <f t="shared" si="0"/>
         <v>1372.31</v>
       </c>
       <c r="I38" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J38" s="5">
-        <f>I38*F38</f>
+        <f t="shared" si="1"/>
         <v>457.43666666666661</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1372.31</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1407.2199999999989</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P38" s="5">
-        <f>N38*F38 + O38</f>
+        <f t="shared" si="14"/>
         <v>457.43666666666661</v>
       </c>
       <c r="Q38" s="10">
@@ -2706,19 +2706,19 @@
         <v>445.17</v>
       </c>
       <c r="R38" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-33.836666666666531</v>
       </c>
       <c r="T38" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U38" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U38" s="5">
-        <f>T38*F38</f>
         <v>457.43666666666661</v>
       </c>
       <c r="W38" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1434.983333333334</v>
       </c>
       <c r="AG38" s="5"/>
@@ -2738,31 +2738,31 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F39" s="1">
-        <f>C39 + D39 + E39</f>
+        <f t="shared" si="0"/>
         <v>1405.77</v>
       </c>
       <c r="I39" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J39" s="5">
-        <f>I39*F39</f>
+        <f t="shared" si="1"/>
         <v>468.59</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1405.77</v>
       </c>
       <c r="L39" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>914.36999999999898</v>
       </c>
       <c r="M39" s="5"/>
       <c r="N39" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P39" s="5">
-        <f>N39*F39 + O39</f>
+        <f t="shared" si="14"/>
         <v>468.59</v>
       </c>
       <c r="Q39" s="10">
@@ -2770,19 +2770,19 @@
         <v>444.33000000000004</v>
       </c>
       <c r="R39" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-58.096666666666465</v>
       </c>
       <c r="T39" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U39" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U39" s="5">
-        <f>T39*F39</f>
         <v>468.59</v>
       </c>
       <c r="W39" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>966.39333333333411</v>
       </c>
       <c r="AG39" s="5"/>
@@ -2802,31 +2802,31 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F40" s="1">
-        <f>C40 + D40 + E40</f>
+        <f t="shared" si="0"/>
         <v>1358.06</v>
       </c>
       <c r="I40" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J40" s="5">
-        <f>I40*F40</f>
+        <f t="shared" si="1"/>
         <v>452.68666666666661</v>
       </c>
       <c r="K40" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1358.06</v>
       </c>
       <c r="L40" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>494.43666666666564</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P40" s="5">
-        <f>N40*F40 + O40</f>
+        <f t="shared" si="14"/>
         <v>452.68666666666661</v>
       </c>
       <c r="Q40" s="10">
@@ -2834,19 +2834,19 @@
         <v>485.44</v>
       </c>
       <c r="R40" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-25.343333333333078</v>
       </c>
       <c r="T40" s="7">
+        <f t="shared" si="6"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="U40" s="5">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="U40" s="5">
-        <f>T40*F40</f>
         <v>452.68666666666661</v>
       </c>
       <c r="W40" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>513.7066666666675</v>
       </c>
       <c r="AG40" s="5"/>
@@ -2866,50 +2866,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F41" s="1">
-        <f>C41 + D41 + E41</f>
+        <f t="shared" ref="F41:F61" si="16">C41 + D41 + E41</f>
         <v>1347.29</v>
       </c>
       <c r="I41" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J41" s="5">
-        <f>I41*F41</f>
+        <f t="shared" ref="J41:J61" si="17">I41*F41</f>
         <v>449.09666666666664</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1347.29</v>
       </c>
       <c r="L41" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-303.75666666666774</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P41" s="5">
-        <f>N41*F41 + O41</f>
+        <f t="shared" si="14"/>
         <v>449.09666666666664</v>
       </c>
       <c r="R41" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-474.43999999999971</v>
       </c>
       <c r="T41" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U41" s="5">
-        <f>T41*F41</f>
+        <f t="shared" ref="U41:U59" si="18">T41*F41</f>
         <v>449.09666666666664</v>
       </c>
       <c r="V41" s="3">
         <v>100</v>
       </c>
       <c r="W41" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>164.61000000000087</v>
       </c>
       <c r="AG41" s="5"/>
@@ -2929,34 +2929,34 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F42" s="1">
-        <f>C42 + D42 + E42</f>
+        <f t="shared" si="16"/>
         <v>1343.1200000000001</v>
       </c>
       <c r="I42" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J42" s="5">
-        <f>I42*F42</f>
+        <f t="shared" si="17"/>
         <v>447.70666666666671</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1358.1200000000001</v>
       </c>
       <c r="L42" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-286.89000000000124</v>
       </c>
       <c r="M42" s="5"/>
       <c r="N42" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O42" s="1">
         <v>15</v>
       </c>
       <c r="P42" s="5">
-        <f>N42*F42 + O42</f>
+        <f t="shared" si="14"/>
         <v>462.70666666666671</v>
       </c>
       <c r="Q42" s="10">
@@ -2964,19 +2964,19 @@
         <v>927.28</v>
       </c>
       <c r="R42" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-9.8666666666664469</v>
       </c>
       <c r="T42" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U42" s="5">
-        <f>T42*F42</f>
+        <f t="shared" si="18"/>
         <v>447.70666666666671</v>
       </c>
       <c r="W42" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-283.09666666666584</v>
       </c>
       <c r="AG42" s="5"/>
@@ -2996,34 +2996,34 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F43" s="1">
-        <f>C43 + D43 + E43</f>
+        <f t="shared" si="16"/>
         <v>1300.3900000000001</v>
       </c>
       <c r="I43" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J43" s="5">
-        <f>I43*F43</f>
+        <f t="shared" si="17"/>
         <v>433.46333333333337</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1315.39</v>
       </c>
       <c r="L43" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1034.2833333333319</v>
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O43" s="1">
         <v>15</v>
       </c>
       <c r="P43" s="5">
-        <f>N43*F43 + O43</f>
+        <f t="shared" si="14"/>
         <v>448.46333333333337</v>
       </c>
       <c r="Q43" s="10">
@@ -3031,22 +3031,22 @@
         <v>449.1</v>
       </c>
       <c r="R43" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-9.2299999999997908</v>
       </c>
       <c r="T43" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U43" s="5">
-        <f>T43*F43</f>
+        <f t="shared" si="18"/>
         <v>433.46333333333337</v>
       </c>
       <c r="V43" s="3">
         <v>1754</v>
       </c>
       <c r="W43" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1037.4400000000007</v>
       </c>
       <c r="AG43" s="5"/>
@@ -3066,53 +3066,53 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F44" s="1">
-        <f>C44 + D44 + E44</f>
+        <f t="shared" si="16"/>
         <v>1279.33</v>
       </c>
       <c r="I44" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J44" s="5">
-        <f>I44*F44</f>
+        <f t="shared" si="17"/>
         <v>426.44333333333327</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1294.33</v>
       </c>
       <c r="L44" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>548.06666666666524</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O44" s="1">
         <v>15</v>
       </c>
       <c r="P44" s="5">
-        <f>N44*F44 + O44</f>
+        <f t="shared" si="14"/>
         <v>441.44333333333327</v>
       </c>
       <c r="Q44" s="10">
         <v>381.67</v>
       </c>
       <c r="R44" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-69.003333333333046</v>
       </c>
       <c r="T44" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U44" s="5">
-        <f>T44*F44</f>
+        <f t="shared" si="18"/>
         <v>426.44333333333327</v>
       </c>
       <c r="W44" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>610.99666666666747</v>
       </c>
       <c r="AG44" s="5"/>
@@ -3132,50 +3132,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F45" s="1">
-        <f>C45 + D45 + E45</f>
+        <f t="shared" si="16"/>
         <v>1274.5899999999999</v>
       </c>
       <c r="I45" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J45" s="5">
-        <f>I45*F45</f>
+        <f t="shared" si="17"/>
         <v>424.86333333333329</v>
       </c>
       <c r="K45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1289.5899999999999</v>
       </c>
       <c r="L45" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-316.66000000000139</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O45" s="1">
         <v>15</v>
       </c>
       <c r="P45" s="5">
-        <f>N45*F45 + O45</f>
+        <f t="shared" si="14"/>
         <v>439.86333333333329</v>
       </c>
       <c r="R45" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-508.86666666666633</v>
       </c>
       <c r="T45" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U45" s="5">
-        <f>T45*F45</f>
+        <f t="shared" si="18"/>
         <v>424.86333333333329</v>
       </c>
       <c r="W45" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>186.13333333333418</v>
       </c>
       <c r="AG45" s="5"/>
@@ -3195,50 +3195,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F46" s="1">
-        <f>C46 + D46 + E46</f>
+        <f t="shared" si="16"/>
         <v>1256.5899999999999</v>
       </c>
       <c r="I46" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J46" s="5">
-        <f>I46*F46</f>
+        <f t="shared" si="17"/>
         <v>418.86333333333329</v>
       </c>
       <c r="K46" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1271.5899999999999</v>
       </c>
       <c r="L46" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1169.3866666666681</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O46" s="1">
         <v>15</v>
       </c>
       <c r="P46" s="5">
-        <f>N46*F46 + O46</f>
+        <f t="shared" si="14"/>
         <v>433.86333333333329</v>
       </c>
       <c r="R46" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-942.72999999999956</v>
       </c>
       <c r="T46" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U46" s="5">
-        <f>T46*F46</f>
+        <f t="shared" si="18"/>
         <v>418.86333333333329</v>
       </c>
       <c r="W46" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-232.72999999999911</v>
       </c>
       <c r="AG46" s="5"/>
@@ -3258,50 +3258,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F47" s="1">
-        <f>C47 + D47 + E47</f>
+        <f t="shared" si="16"/>
         <v>1358.66</v>
       </c>
       <c r="I47" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J47" s="5">
-        <f>I47*F47</f>
+        <f t="shared" si="17"/>
         <v>452.88666666666666</v>
       </c>
       <c r="K47" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1358.66</v>
       </c>
       <c r="L47" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-685.36000000000126</v>
       </c>
       <c r="M47" s="5"/>
       <c r="N47" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P47" s="5">
-        <f>N47*F47 + O47</f>
+        <f t="shared" si="14"/>
         <v>452.88666666666666</v>
       </c>
       <c r="Q47" s="10">
         <v>1389.8</v>
       </c>
       <c r="R47" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-5.8166666666663787</v>
       </c>
       <c r="T47" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U47" s="5">
-        <f>T47*F47</f>
+        <f t="shared" si="18"/>
         <v>452.88666666666666</v>
       </c>
       <c r="W47" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-685.61666666666576</v>
       </c>
       <c r="AG47" s="5"/>
@@ -3321,50 +3321,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F48" s="1">
-        <f>C48 + D48 + E48</f>
+        <f t="shared" si="16"/>
         <v>1360.66</v>
       </c>
       <c r="I48" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J48" s="5">
-        <f>I48*F48</f>
+        <f t="shared" si="17"/>
         <v>453.55333333333334</v>
       </c>
       <c r="K48" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1360.66</v>
       </c>
       <c r="L48" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1167.6066666666679</v>
       </c>
       <c r="M48" s="5"/>
       <c r="N48" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P48" s="5">
-        <f>N48*F48 + O48</f>
+        <f t="shared" si="14"/>
         <v>453.55333333333334</v>
       </c>
       <c r="Q48" s="10">
         <v>424.86</v>
       </c>
       <c r="R48" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-34.509999999999707</v>
       </c>
       <c r="T48" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U48" s="5">
-        <f>T48*F48</f>
+        <f t="shared" si="18"/>
         <v>453.55333333333334</v>
       </c>
       <c r="W48" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1139.1699999999992</v>
       </c>
       <c r="AG48" s="5"/>
@@ -3384,50 +3384,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F49" s="1">
-        <f>C49 + D49 + E49</f>
+        <f t="shared" si="16"/>
         <v>1372.91</v>
       </c>
       <c r="I49" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J49" s="5">
-        <f>I49*F49</f>
+        <f t="shared" si="17"/>
         <v>457.63666666666666</v>
       </c>
       <c r="K49" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1372.91</v>
       </c>
       <c r="L49" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1083.1199999999985</v>
       </c>
       <c r="M49" s="5"/>
       <c r="N49" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P49" s="5">
-        <f>N49*F49 + O49</f>
+        <f t="shared" si="14"/>
         <v>457.63666666666666</v>
       </c>
       <c r="R49" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-492.14666666666636</v>
       </c>
       <c r="T49" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U49" s="5">
-        <f>T49*F49</f>
+        <f t="shared" si="18"/>
         <v>457.63666666666666</v>
       </c>
       <c r="V49" s="3">
         <v>3166</v>
       </c>
       <c r="W49" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1569.1933333333341</v>
       </c>
       <c r="AG49" s="5"/>
@@ -3450,50 +3450,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F50" s="1">
-        <f>C50 + D50 + E50</f>
+        <f t="shared" si="16"/>
         <v>1364.18</v>
       </c>
       <c r="I50" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J50" s="5">
-        <f>I50*F50</f>
+        <f t="shared" si="17"/>
         <v>454.72666666666669</v>
       </c>
       <c r="K50" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1364.18</v>
       </c>
       <c r="L50" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1080.1066666666652</v>
       </c>
       <c r="M50" s="5"/>
       <c r="N50" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P50" s="5">
-        <f>N50*F50 + O50</f>
+        <f t="shared" si="14"/>
         <v>454.72666666666669</v>
       </c>
       <c r="Q50" s="10">
         <v>906.44</v>
       </c>
       <c r="R50" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-40.433333333332939</v>
       </c>
       <c r="T50" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U50" s="5">
-        <f>T50*F50</f>
+        <f t="shared" si="18"/>
         <v>454.72666666666669</v>
       </c>
       <c r="W50" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1114.4666666666674</v>
       </c>
       <c r="AG50" s="5"/>
@@ -3513,50 +3513,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F51" s="1">
-        <f>C51 + D51 + E51</f>
+        <f t="shared" si="16"/>
         <v>1375.79</v>
       </c>
       <c r="I51" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J51" s="5">
-        <f>I51*F51</f>
+        <f t="shared" si="17"/>
         <v>458.59666666666664</v>
       </c>
       <c r="K51" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1375.79</v>
       </c>
       <c r="L51" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>620.55333333333192</v>
       </c>
       <c r="M51" s="5"/>
       <c r="N51" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P51" s="5">
-        <f>N51*F51 + O51</f>
+        <f t="shared" si="14"/>
         <v>458.59666666666664</v>
       </c>
       <c r="Q51" s="10">
         <v>457.64</v>
       </c>
       <c r="R51" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-41.389999999999588</v>
       </c>
       <c r="T51" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U51" s="5">
-        <f>T51*F51</f>
+        <f t="shared" si="18"/>
         <v>458.59666666666664</v>
       </c>
       <c r="W51" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>655.8700000000008</v>
       </c>
       <c r="AG51" s="5"/>
@@ -3576,50 +3576,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F52" s="1">
-        <f>C52 + D52 + E52</f>
+        <f t="shared" si="16"/>
         <v>1393.16</v>
       </c>
       <c r="I52" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J52" s="5">
-        <f>I52*F52</f>
+        <f t="shared" si="17"/>
         <v>464.38666666666666</v>
       </c>
       <c r="K52" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1393.16</v>
       </c>
       <c r="L52" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>146.50999999999851</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P52" s="5">
-        <f>N52*F52 + O52</f>
+        <f t="shared" si="14"/>
         <v>464.38666666666666</v>
       </c>
       <c r="Q52" s="10">
         <v>454.73</v>
       </c>
       <c r="R52" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-51.046666666666226</v>
       </c>
       <c r="T52" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U52" s="5">
-        <f>T52*F52</f>
+        <f t="shared" si="18"/>
         <v>464.38666666666666</v>
       </c>
       <c r="W52" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>191.48333333333414</v>
       </c>
       <c r="AG52" s="5"/>
@@ -3639,50 +3639,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F53" s="1">
-        <f>C53 + D53 + E53</f>
+        <f t="shared" si="16"/>
         <v>1210.99</v>
       </c>
       <c r="I53" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J53" s="5">
-        <f>I53*F53</f>
+        <f t="shared" si="17"/>
         <v>403.6633333333333</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1210.99</v>
       </c>
       <c r="L53" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-202.22666666666811</v>
       </c>
       <c r="M53" s="5"/>
       <c r="N53" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P53" s="5">
-        <f>N53*F53 + O53</f>
+        <f t="shared" si="14"/>
         <v>403.6633333333333</v>
       </c>
       <c r="Q53" s="10">
         <v>458.59</v>
       </c>
       <c r="R53" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.8800000000004502</v>
       </c>
       <c r="T53" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U53" s="5">
-        <f>T53*F53</f>
+        <f t="shared" si="18"/>
         <v>403.6633333333333</v>
       </c>
       <c r="W53" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-212.17999999999915</v>
       </c>
       <c r="AG53" s="5"/>
@@ -3702,50 +3702,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F54" s="1">
-        <f>C54 + D54 + E54</f>
+        <f t="shared" si="16"/>
         <v>1210.99</v>
       </c>
       <c r="I54" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J54" s="5">
-        <f>I54*F54</f>
+        <f t="shared" si="17"/>
         <v>403.6633333333333</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1210.99</v>
       </c>
       <c r="L54" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-545.16333333333478</v>
       </c>
       <c r="M54" s="5"/>
       <c r="N54" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P54" s="5">
-        <f>N54*F54 + O54</f>
+        <f t="shared" si="14"/>
         <v>403.6633333333333</v>
       </c>
       <c r="Q54" s="10">
         <v>464.39</v>
       </c>
       <c r="R54" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>64.606666666667138</v>
       </c>
       <c r="T54" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U54" s="5">
-        <f>T54*F54</f>
+        <f t="shared" si="18"/>
         <v>403.6633333333333</v>
       </c>
       <c r="W54" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-615.84333333333245</v>
       </c>
       <c r="AG54" s="5"/>
@@ -3765,50 +3765,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F55" s="1">
-        <f>C55 + D55 + E55</f>
+        <f t="shared" si="16"/>
         <v>1563.34</v>
       </c>
       <c r="I55" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J55" s="5">
-        <f>I55*F55</f>
+        <f t="shared" si="17"/>
         <v>521.11333333333323</v>
       </c>
       <c r="K55" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1563.34</v>
       </c>
       <c r="L55" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-1183.7300000000016</v>
       </c>
       <c r="M55" s="5"/>
       <c r="N55" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P55" s="5">
-        <f>N55*F55 + O55</f>
+        <f t="shared" si="14"/>
         <v>521.11333333333323</v>
       </c>
       <c r="Q55" s="10">
         <v>403.66</v>
       </c>
       <c r="R55" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-52.846666666666067</v>
       </c>
       <c r="T55" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U55" s="5">
-        <f>T55*F55</f>
+        <f t="shared" si="18"/>
         <v>521.11333333333323</v>
       </c>
       <c r="W55" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-1136.9566666666656</v>
       </c>
       <c r="AG55" s="5"/>
@@ -3828,53 +3828,53 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F56" s="1">
-        <f>C56 + D56 + E56</f>
+        <f t="shared" si="16"/>
         <v>1319.31</v>
       </c>
       <c r="I56" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J56" s="5">
-        <f>I56*F56</f>
+        <f t="shared" si="17"/>
         <v>439.77</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1319.31</v>
       </c>
       <c r="L56" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>100.39999999999827</v>
       </c>
       <c r="M56" s="5"/>
       <c r="N56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P56" s="5">
-        <f>N56*F56 + O56</f>
+        <f t="shared" si="14"/>
         <v>439.77</v>
       </c>
       <c r="Q56" s="10">
         <v>403.67</v>
       </c>
       <c r="R56" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-88.946666666666033</v>
       </c>
       <c r="T56" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U56" s="5">
-        <f>T56*F56</f>
+        <f t="shared" si="18"/>
         <v>439.77</v>
       </c>
       <c r="V56" s="3">
         <v>1760</v>
       </c>
       <c r="W56" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>183.27333333333445</v>
       </c>
       <c r="AG56" s="5"/>
@@ -3894,50 +3894,50 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F57" s="1">
-        <f>C57 + D57 + E57</f>
+        <f t="shared" si="16"/>
         <v>1315.96</v>
       </c>
       <c r="I57" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J57" s="5">
-        <f>I57*F57</f>
+        <f t="shared" si="17"/>
         <v>438.65333333333331</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1315.96</v>
       </c>
       <c r="L57" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-255.79666666666844</v>
       </c>
       <c r="M57" s="5"/>
       <c r="N57" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P57" s="5">
-        <f>N57*F57 + O57</f>
+        <f t="shared" si="14"/>
         <v>438.65333333333331</v>
       </c>
       <c r="Q57" s="10">
         <v>521.11</v>
       </c>
       <c r="R57" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-6.489999999999327</v>
       </c>
       <c r="T57" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U57" s="5">
-        <f>T57*F57</f>
+        <f t="shared" si="18"/>
         <v>438.65333333333331</v>
       </c>
       <c r="W57" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-255.37999999999886</v>
       </c>
       <c r="AG57" s="5"/>
@@ -3957,18 +3957,18 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F58" s="1">
-        <f>C58 + D58 + E58</f>
+        <f t="shared" si="16"/>
         <v>1341.83</v>
       </c>
       <c r="I58" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J58" s="5">
-        <f>I58*F58</f>
+        <f t="shared" si="17"/>
         <v>447.27666666666664</v>
       </c>
       <c r="K58" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1341.83</v>
       </c>
       <c r="L58" s="5">
@@ -3977,33 +3977,33 @@
       </c>
       <c r="M58" s="5"/>
       <c r="N58" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P58" s="5">
-        <f>N58*F58 + O58</f>
+        <f t="shared" si="14"/>
         <v>447.27666666666664</v>
       </c>
       <c r="Q58" s="10">
         <v>439.77</v>
       </c>
       <c r="R58" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>-13.996666666665988</v>
       </c>
       <c r="T58" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U58" s="5">
-        <f>T58*F58</f>
+        <f t="shared" si="18"/>
         <v>447.27666666666664</v>
       </c>
       <c r="V58" s="3">
         <v>440</v>
       </c>
       <c r="W58" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-262.6566666666655</v>
       </c>
       <c r="AG58" s="5"/>
@@ -4023,51 +4023,54 @@
         <v>65.989999999999995</v>
       </c>
       <c r="F59" s="1">
-        <f>C59 + D59 + E59</f>
+        <f t="shared" si="16"/>
         <v>1264.02</v>
       </c>
       <c r="I59" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="J59" s="5">
-        <f>I59*F59</f>
+        <f t="shared" si="17"/>
         <v>421.34</v>
       </c>
       <c r="K59" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>-1264.02</v>
       </c>
       <c r="L59" s="5">
-        <f t="shared" si="1"/>
-        <v>-674.61000000000183</v>
+        <f t="shared" si="5"/>
+        <v>-174.61000000000183</v>
       </c>
       <c r="M59" s="5"/>
       <c r="N59" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="P59" s="5">
-        <f>N59*F59 + O59</f>
+        <f t="shared" si="14"/>
         <v>421.34</v>
       </c>
       <c r="Q59" s="10">
         <v>438.65</v>
       </c>
       <c r="R59" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>3.3133333333340147</v>
       </c>
       <c r="T59" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="U59" s="5">
-        <f>T59*F59</f>
+        <f t="shared" si="18"/>
         <v>421.34</v>
       </c>
+      <c r="V59" s="3">
+        <v>500</v>
+      </c>
       <c r="W59" s="5">
-        <f t="shared" si="3"/>
-        <v>-683.99666666666553</v>
+        <f t="shared" si="7"/>
+        <v>-183.99666666666553</v>
       </c>
       <c r="AG59" s="5"/>
       <c r="BK59" s="3"/>
@@ -4079,28 +4082,31 @@
       <c r="C60" s="1">
         <v>1145</v>
       </c>
+      <c r="D60" s="1">
+        <v>117.83</v>
+      </c>
       <c r="E60" s="1">
         <v>65.989999999999995</v>
       </c>
       <c r="F60" s="1">
-        <f>C60 + D60 + E60</f>
-        <v>1210.99</v>
+        <f t="shared" si="16"/>
+        <v>1328.82</v>
       </c>
       <c r="I60" s="8">
         <f>35000/(35000+24000)</f>
         <v>0.59322033898305082</v>
       </c>
       <c r="J60" s="5">
-        <f>I60*F60</f>
-        <v>718.3838983050847</v>
+        <f t="shared" si="17"/>
+        <v>788.2830508474575</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" si="0"/>
-        <v>-1210.99</v>
+        <f t="shared" si="4"/>
+        <v>-1328.82</v>
       </c>
       <c r="L60" s="5">
-        <f t="shared" si="1"/>
-        <v>-621.37610169491711</v>
+        <f t="shared" si="5"/>
+        <v>-169.31694915254411</v>
       </c>
       <c r="M60" s="5"/>
       <c r="N60" s="7">
@@ -4108,15 +4114,15 @@
         <v>0.40677966101694918</v>
       </c>
       <c r="P60" s="5">
-        <f>N60*F60 + O60</f>
-        <v>492.60610169491531</v>
+        <f t="shared" si="14"/>
+        <v>540.53694915254243</v>
       </c>
       <c r="Q60" s="10">
-        <v>545.84</v>
+        <v>545.83000000000004</v>
       </c>
       <c r="R60" s="5">
-        <f t="shared" si="9"/>
-        <v>56.547231638418737</v>
+        <f t="shared" si="15"/>
+        <v>8.6063841807916788</v>
       </c>
       <c r="AG60" s="5"/>
     </row>
@@ -4126,6 +4132,41 @@
       </c>
       <c r="C61" s="1">
         <v>1145</v>
+      </c>
+      <c r="E61" s="1">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="F61" s="1">
+        <f t="shared" si="16"/>
+        <v>1210.99</v>
+      </c>
+      <c r="I61" s="8">
+        <f>35000/(35000+24000)</f>
+        <v>0.59322033898305082</v>
+      </c>
+      <c r="J61" s="5">
+        <f t="shared" si="17"/>
+        <v>718.3838983050847</v>
+      </c>
+      <c r="K61" s="2">
+        <f t="shared" si="4"/>
+        <v>-1210.99</v>
+      </c>
+      <c r="L61" s="5">
+        <f t="shared" si="5"/>
+        <v>-661.92305084745942</v>
+      </c>
+      <c r="N61" s="7">
+        <f>1-I61</f>
+        <v>0.40677966101694918</v>
+      </c>
+      <c r="P61" s="5">
+        <f t="shared" si="14"/>
+        <v>492.60610169491531</v>
+      </c>
+      <c r="R61" s="5">
+        <f t="shared" si="15"/>
+        <v>-483.99971751412363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>